<commit_message>
chore(humedad): reinforce UND column and upload updated template
</commit_message>
<xml_diff>
--- a/app/templates/Template_Humedad.xlsx
+++ b/app/templates/Template_Humedad.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\crmnew\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\crmnew\api-geofal-crm\app\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{02DC1C9E-F741-4F2E-A4DA-B4C12488ACF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40ABFF1-F9A4-4FE4-BAFB-15FF1B5D5AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="723" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="74">
   <si>
     <t>FC</t>
   </si>
@@ -256,64 +256,20 @@
     <t>Versión: 04 (01-12-2022)</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>WEB: www.geofal.com.pe   E-MAIL: laboratorio@geofal.com.pe                                                                                                                                                                         Av. Marañon 763, Los Olivos-Lima / Teléfono  01 754-3070</t>
-  </si>
-  <si>
-    <t>TM</t>
-  </si>
-  <si>
-    <t>MASA MINIMA</t>
-  </si>
-  <si>
-    <t>(in.)</t>
-  </si>
-  <si>
-    <t>(g)</t>
-  </si>
-  <si>
-    <t>1/2</t>
-  </si>
-  <si>
-    <t>3/8</t>
-  </si>
-  <si>
-    <t>N°4</t>
-  </si>
-  <si>
-    <t>N°10</t>
-  </si>
-  <si>
-    <t>Tamaño máximo TM:</t>
-  </si>
-  <si>
-    <t>Cantidad mínima:</t>
-  </si>
-  <si>
-    <t>EQP-0046</t>
-  </si>
-  <si>
-    <t>EQP-0045</t>
-  </si>
-  <si>
-    <t>EQP-0049</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="000"/>
     <numFmt numFmtId="166" formatCode="0\ &quot;/ CO-06&quot;"/>
     <numFmt numFmtId="167" formatCode="&quot;FORMATO F-LEM-P-SU-11.01&quot;"/>
-    <numFmt numFmtId="168" formatCode="#,##0.0"/>
-    <numFmt numFmtId="169" formatCode="0\ &quot;g&quot;"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -442,22 +398,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFC00000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -467,12 +409,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -722,7 +658,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="158">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1053,53 +989,103 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="12" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="12" fontId="22" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1108,10 +1094,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -1152,92 +1134,7 @@
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1252,13 +1149,7 @@
     <cellStyle name="Normal 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Normal_ENSAYOS" xfId="3" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -2659,7 +2550,7 @@
   <dimension ref="A1:W63"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="N14" sqref="N14:Q32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.33203125" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2682,7 +2573,7 @@
     <col min="16" max="16384" width="10.33203125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13"/>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -2696,7 +2587,7 @@
       <c r="K1" s="16"/>
       <c r="L1" s="17"/>
     </row>
-    <row r="2" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19"/>
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
@@ -2708,7 +2599,7 @@
       <c r="I2" s="21"/>
       <c r="L2" s="22"/>
     </row>
-    <row r="3" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
       <c r="B3" s="20"/>
       <c r="C3" s="20"/>
@@ -2720,7 +2611,7 @@
       <c r="I3" s="21"/>
       <c r="L3" s="22"/>
     </row>
-    <row r="4" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
       <c r="B4" s="20"/>
       <c r="C4" s="20"/>
@@ -2732,7 +2623,7 @@
       <c r="I4" s="21"/>
       <c r="L4" s="22"/>
     </row>
-    <row r="5" spans="1:17" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23"/>
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
@@ -2746,7 +2637,7 @@
       <c r="K5" s="24"/>
       <c r="L5" s="25"/>
     </row>
-    <row r="6" spans="1:17" ht="6.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="6.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="26"/>
       <c r="B6" s="26"/>
       <c r="C6" s="26"/>
@@ -2760,39 +2651,39 @@
       <c r="K6" s="26"/>
       <c r="L6" s="26"/>
     </row>
-    <row r="7" spans="1:17" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="135" t="s">
+    <row r="7" spans="1:13" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="125" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="135"/>
-      <c r="C7" s="135"/>
-      <c r="D7" s="135"/>
-      <c r="E7" s="135"/>
-      <c r="F7" s="135"/>
-      <c r="G7" s="135"/>
-      <c r="H7" s="135"/>
-      <c r="I7" s="135"/>
-      <c r="J7" s="135"/>
-      <c r="K7" s="135"/>
-      <c r="L7" s="135"/>
-    </row>
-    <row r="8" spans="1:17" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="136" t="s">
+      <c r="B7" s="125"/>
+      <c r="C7" s="125"/>
+      <c r="D7" s="125"/>
+      <c r="E7" s="125"/>
+      <c r="F7" s="125"/>
+      <c r="G7" s="125"/>
+      <c r="H7" s="125"/>
+      <c r="I7" s="125"/>
+      <c r="J7" s="125"/>
+      <c r="K7" s="125"/>
+      <c r="L7" s="125"/>
+    </row>
+    <row r="8" spans="1:13" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="126" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="136"/>
-      <c r="C8" s="136"/>
-      <c r="D8" s="136"/>
-      <c r="E8" s="136"/>
-      <c r="F8" s="136"/>
-      <c r="G8" s="136"/>
-      <c r="H8" s="136"/>
-      <c r="I8" s="136"/>
-      <c r="J8" s="136"/>
-      <c r="K8" s="136"/>
-      <c r="L8" s="136"/>
-    </row>
-    <row r="9" spans="1:17" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="126"/>
+      <c r="C8" s="126"/>
+      <c r="D8" s="126"/>
+      <c r="E8" s="126"/>
+      <c r="F8" s="126"/>
+      <c r="G8" s="126"/>
+      <c r="H8" s="126"/>
+      <c r="I8" s="126"/>
+      <c r="J8" s="126"/>
+      <c r="K8" s="126"/>
+      <c r="L8" s="126"/>
+    </row>
+    <row r="9" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27"/>
       <c r="B9" s="27"/>
       <c r="C9" s="27"/>
@@ -2806,7 +2697,7 @@
       <c r="K9" s="27"/>
       <c r="L9" s="27"/>
     </row>
-    <row r="10" spans="1:17" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="27"/>
       <c r="B10" s="27"/>
       <c r="C10" s="27"/>
@@ -2820,7 +2711,7 @@
       <c r="K10" s="27"/>
       <c r="L10" s="27"/>
     </row>
-    <row r="11" spans="1:17" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="27"/>
       <c r="B11" s="27"/>
       <c r="C11" s="27"/>
@@ -2834,7 +2725,7 @@
       <c r="K11" s="27"/>
       <c r="L11" s="27"/>
     </row>
-    <row r="12" spans="1:17" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="27"/>
       <c r="B12" s="27"/>
       <c r="C12" s="27"/>
@@ -2848,7 +2739,7 @@
       <c r="K12" s="27"/>
       <c r="L12" s="27"/>
     </row>
-    <row r="13" spans="1:17" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="28"/>
       <c r="B13" s="29"/>
       <c r="C13" s="30"/>
@@ -2863,41 +2754,41 @@
       <c r="L13" s="31"/>
       <c r="M13" s="32"/>
     </row>
-    <row r="14" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="137" t="s">
+    <row r="14" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="127" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="138"/>
-      <c r="C14" s="138"/>
-      <c r="D14" s="138"/>
-      <c r="E14" s="138"/>
-      <c r="F14" s="138"/>
-      <c r="G14" s="138"/>
-      <c r="H14" s="138"/>
-      <c r="I14" s="138"/>
-      <c r="J14" s="138"/>
-      <c r="K14" s="138"/>
-      <c r="L14" s="139"/>
+      <c r="B14" s="128"/>
+      <c r="C14" s="128"/>
+      <c r="D14" s="128"/>
+      <c r="E14" s="128"/>
+      <c r="F14" s="128"/>
+      <c r="G14" s="128"/>
+      <c r="H14" s="128"/>
+      <c r="I14" s="128"/>
+      <c r="J14" s="128"/>
+      <c r="K14" s="128"/>
+      <c r="L14" s="129"/>
       <c r="M14" s="32"/>
     </row>
-    <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="147" t="s">
+    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="119" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="148"/>
-      <c r="C15" s="148"/>
-      <c r="D15" s="148"/>
-      <c r="E15" s="148"/>
-      <c r="F15" s="148"/>
-      <c r="G15" s="148"/>
-      <c r="H15" s="148"/>
-      <c r="I15" s="148"/>
-      <c r="J15" s="148"/>
-      <c r="K15" s="148"/>
-      <c r="L15" s="149"/>
+      <c r="B15" s="120"/>
+      <c r="C15" s="120"/>
+      <c r="D15" s="120"/>
+      <c r="E15" s="120"/>
+      <c r="F15" s="120"/>
+      <c r="G15" s="120"/>
+      <c r="H15" s="120"/>
+      <c r="I15" s="120"/>
+      <c r="J15" s="120"/>
+      <c r="K15" s="120"/>
+      <c r="L15" s="121"/>
       <c r="M15" s="32"/>
     </row>
-    <row r="16" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="33"/>
       <c r="B16" s="34"/>
       <c r="C16" s="35"/>
@@ -2911,36 +2802,24 @@
       <c r="K16" s="34"/>
       <c r="L16" s="36"/>
       <c r="M16" s="32"/>
-      <c r="N16" s="110" t="s">
-        <v>83</v>
-      </c>
-      <c r="O16" s="111"/>
-      <c r="P16" s="112" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q16" s="113"/>
-    </row>
-    <row r="17" spans="1:23" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="140" t="s">
+    </row>
+    <row r="17" spans="1:19" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="130" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="141"/>
-      <c r="C17" s="141"/>
-      <c r="D17" s="141"/>
-      <c r="E17" s="141"/>
-      <c r="F17" s="141"/>
-      <c r="G17" s="141"/>
-      <c r="H17" s="141"/>
-      <c r="I17" s="141"/>
+      <c r="B17" s="131"/>
+      <c r="C17" s="131"/>
+      <c r="D17" s="131"/>
+      <c r="E17" s="131"/>
+      <c r="F17" s="131"/>
+      <c r="G17" s="131"/>
+      <c r="H17" s="131"/>
+      <c r="I17" s="131"/>
       <c r="J17" s="37"/>
       <c r="K17" s="37"/>
       <c r="L17" s="38"/>
-      <c r="N17" s="113"/>
-      <c r="O17" s="113"/>
-      <c r="P17" s="113"/>
-      <c r="Q17" s="113"/>
-    </row>
-    <row r="18" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="39" t="s">
         <v>34</v>
       </c>
@@ -2955,20 +2834,8 @@
       <c r="J18" s="102"/>
       <c r="K18" s="37"/>
       <c r="L18" s="38"/>
-      <c r="N18" s="110" t="s">
-        <v>84</v>
-      </c>
-      <c r="O18" s="111"/>
-      <c r="P18" s="114">
-        <f>+INDEX(N22:O31,MATCH(P16,N22:N31,0),2)</f>
-        <v>250</v>
-      </c>
-      <c r="Q18" s="115" t="str">
-        <f>+IF((I33-I36)&gt;P18,"Cumple","No Cumple")</f>
-        <v>No Cumple</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="39" t="s">
         <v>35</v>
       </c>
@@ -2984,7 +2851,7 @@
       <c r="K19" s="37"/>
       <c r="L19" s="38"/>
     </row>
-    <row r="20" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="39" t="s">
         <v>52</v>
       </c>
@@ -2999,14 +2866,8 @@
       <c r="J20" s="102"/>
       <c r="K20" s="37"/>
       <c r="L20" s="38"/>
-      <c r="N20" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="O20" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="39" t="s">
         <v>36</v>
       </c>
@@ -3021,14 +2882,8 @@
       <c r="J21" s="102"/>
       <c r="K21" s="37"/>
       <c r="L21" s="38"/>
-      <c r="N21" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="O21" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="41" t="s">
         <v>47</v>
       </c>
@@ -3043,14 +2898,8 @@
       <c r="J22" s="37"/>
       <c r="K22" s="37"/>
       <c r="L22" s="38"/>
-      <c r="N22" s="104">
-        <v>3</v>
-      </c>
-      <c r="O22" s="104">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="42"/>
       <c r="B23" s="43"/>
       <c r="C23" s="43"/>
@@ -3063,20 +2912,14 @@
       <c r="J23" s="37"/>
       <c r="K23" s="37"/>
       <c r="L23" s="38"/>
-      <c r="N23" s="105">
-        <v>2.5</v>
-      </c>
-      <c r="O23" s="104">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="140" t="s">
+    </row>
+    <row r="24" spans="1:19" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="130" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="141"/>
-      <c r="C24" s="141"/>
-      <c r="D24" s="141"/>
+      <c r="B24" s="131"/>
+      <c r="C24" s="131"/>
+      <c r="D24" s="131"/>
       <c r="E24" s="43"/>
       <c r="F24" s="43"/>
       <c r="G24" s="43"/>
@@ -3085,101 +2928,71 @@
       <c r="J24" s="37"/>
       <c r="K24" s="37"/>
       <c r="L24" s="38"/>
-      <c r="N24" s="106">
-        <v>2</v>
-      </c>
-      <c r="O24" s="104">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="142" t="s">
+    </row>
+    <row r="25" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="123" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="142"/>
-      <c r="C25" s="142"/>
-      <c r="D25" s="142"/>
-      <c r="E25" s="143"/>
-      <c r="F25" s="143"/>
+      <c r="B25" s="123"/>
+      <c r="C25" s="123"/>
+      <c r="D25" s="123"/>
+      <c r="E25" s="124"/>
+      <c r="F25" s="124"/>
       <c r="G25" s="44"/>
-      <c r="H25" s="144" t="s">
+      <c r="H25" s="116" t="s">
         <v>42</v>
       </c>
-      <c r="I25" s="145"/>
-      <c r="J25" s="146"/>
+      <c r="I25" s="117"/>
+      <c r="J25" s="118"/>
       <c r="K25" s="45"/>
       <c r="L25" s="38"/>
-      <c r="N25" s="105">
-        <v>1.5</v>
-      </c>
-      <c r="O25" s="104">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="142" t="s">
+    </row>
+    <row r="26" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="123" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="142"/>
-      <c r="C26" s="142"/>
-      <c r="D26" s="142"/>
-      <c r="E26" s="143"/>
-      <c r="F26" s="143"/>
+      <c r="B26" s="123"/>
+      <c r="C26" s="123"/>
+      <c r="D26" s="123"/>
+      <c r="E26" s="124"/>
+      <c r="F26" s="124"/>
       <c r="G26" s="44"/>
-      <c r="H26" s="144" t="s">
+      <c r="H26" s="116" t="s">
         <v>31</v>
       </c>
-      <c r="I26" s="146"/>
+      <c r="I26" s="118"/>
       <c r="J26" s="103"/>
       <c r="K26" s="46"/>
       <c r="L26" s="38"/>
-      <c r="N26" s="106">
-        <v>1</v>
-      </c>
-      <c r="O26" s="104">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:23" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="142" t="s">
+    </row>
+    <row r="27" spans="1:19" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="123" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="142"/>
-      <c r="C27" s="142"/>
-      <c r="D27" s="142"/>
-      <c r="E27" s="143"/>
-      <c r="F27" s="143"/>
+      <c r="B27" s="123"/>
+      <c r="C27" s="123"/>
+      <c r="D27" s="123"/>
+      <c r="E27" s="124"/>
+      <c r="F27" s="124"/>
       <c r="G27" s="44"/>
-      <c r="H27" s="144" t="s">
+      <c r="H27" s="116" t="s">
         <v>32</v>
       </c>
-      <c r="I27" s="146"/>
+      <c r="I27" s="118"/>
       <c r="J27" s="103"/>
       <c r="K27" s="46"/>
       <c r="L27" s="38"/>
       <c r="M27" s="32"/>
-      <c r="N27" s="105">
-        <v>0.75</v>
-      </c>
-      <c r="O27" s="104">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:19" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="47"/>
       <c r="B28" s="48"/>
       <c r="C28" s="48"/>
       <c r="D28" s="49"/>
       <c r="L28" s="50"/>
       <c r="M28" s="32"/>
-      <c r="N28" s="107" t="s">
-        <v>79</v>
-      </c>
-      <c r="O28" s="104">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="29" spans="1:23" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:19" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="51"/>
       <c r="B29" s="52"/>
       <c r="C29" s="52"/>
@@ -3193,113 +3006,87 @@
       <c r="K29" s="54"/>
       <c r="L29" s="55"/>
       <c r="M29" s="32"/>
-      <c r="N29" s="107" t="s">
-        <v>80</v>
-      </c>
-      <c r="O29" s="104">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="56"/>
-      <c r="B30" s="154" t="s">
+      <c r="B30" s="115" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="154"/>
-      <c r="D30" s="154"/>
-      <c r="E30" s="154"/>
-      <c r="F30" s="154"/>
-      <c r="G30" s="154"/>
+      <c r="C30" s="115"/>
+      <c r="D30" s="115"/>
+      <c r="E30" s="115"/>
+      <c r="F30" s="115"/>
+      <c r="G30" s="115"/>
       <c r="H30" s="57" t="s">
         <v>44</v>
       </c>
       <c r="I30" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="J30" s="150"/>
-      <c r="K30" s="150"/>
+      <c r="J30" s="122"/>
+      <c r="K30" s="122"/>
       <c r="L30" s="58"/>
       <c r="M30" s="32"/>
-      <c r="N30" s="106" t="s">
-        <v>81</v>
-      </c>
-      <c r="O30" s="104">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="59"/>
       <c r="B31" s="60">
         <v>1</v>
       </c>
-      <c r="C31" s="151" t="s">
+      <c r="C31" s="110" t="s">
         <v>17</v>
       </c>
-      <c r="D31" s="152"/>
-      <c r="E31" s="152"/>
-      <c r="F31" s="152"/>
-      <c r="G31" s="153"/>
+      <c r="D31" s="111"/>
+      <c r="E31" s="111"/>
+      <c r="F31" s="111"/>
+      <c r="G31" s="112"/>
       <c r="H31" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="I31" s="118">
-        <v>1</v>
-      </c>
+      <c r="I31" s="106"/>
       <c r="J31" s="62"/>
       <c r="K31" s="62"/>
       <c r="L31" s="63"/>
       <c r="M31" s="32"/>
-      <c r="N31" s="106" t="s">
-        <v>82</v>
-      </c>
-      <c r="O31" s="104">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:23" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="59"/>
       <c r="B32" s="64">
         <v>2</v>
       </c>
-      <c r="C32" s="151" t="s">
+      <c r="C32" s="110" t="s">
         <v>39</v>
       </c>
-      <c r="D32" s="152"/>
-      <c r="E32" s="152"/>
-      <c r="F32" s="152"/>
-      <c r="G32" s="153"/>
+      <c r="D32" s="111"/>
+      <c r="E32" s="111"/>
+      <c r="F32" s="111"/>
+      <c r="G32" s="112"/>
       <c r="H32" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="I32" s="116"/>
+      <c r="I32" s="104"/>
       <c r="J32" s="62"/>
       <c r="K32" s="62"/>
       <c r="L32" s="63"/>
       <c r="M32" s="32"/>
-      <c r="N32" s="108" t="s">
-        <v>73</v>
-      </c>
-      <c r="O32" s="109" t="s">
-        <v>73</v>
-      </c>
-      <c r="W32" s="66"/>
+      <c r="S32" s="66"/>
     </row>
     <row r="33" spans="1:23" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="59"/>
       <c r="B33" s="64">
         <v>3</v>
       </c>
-      <c r="C33" s="151" t="s">
+      <c r="C33" s="110" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="152"/>
-      <c r="E33" s="152"/>
-      <c r="F33" s="152"/>
-      <c r="G33" s="153"/>
+      <c r="D33" s="111"/>
+      <c r="E33" s="111"/>
+      <c r="F33" s="111"/>
+      <c r="G33" s="112"/>
       <c r="H33" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="I33" s="116"/>
+      <c r="I33" s="104"/>
       <c r="J33" s="62"/>
       <c r="K33" s="62"/>
       <c r="L33" s="67"/>
@@ -3311,17 +3098,17 @@
       <c r="B34" s="60">
         <v>4</v>
       </c>
-      <c r="C34" s="151" t="s">
+      <c r="C34" s="110" t="s">
         <v>61</v>
       </c>
-      <c r="D34" s="152"/>
-      <c r="E34" s="152"/>
-      <c r="F34" s="152"/>
-      <c r="G34" s="153"/>
+      <c r="D34" s="111"/>
+      <c r="E34" s="111"/>
+      <c r="F34" s="111"/>
+      <c r="G34" s="112"/>
       <c r="H34" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="I34" s="116"/>
+      <c r="I34" s="104"/>
       <c r="J34" s="62"/>
       <c r="K34" s="62"/>
       <c r="L34" s="67"/>
@@ -3335,17 +3122,17 @@
       <c r="B35" s="64">
         <v>5</v>
       </c>
-      <c r="C35" s="151" t="s">
+      <c r="C35" s="110" t="s">
         <v>62</v>
       </c>
-      <c r="D35" s="152"/>
-      <c r="E35" s="152"/>
-      <c r="F35" s="152"/>
-      <c r="G35" s="153"/>
+      <c r="D35" s="111"/>
+      <c r="E35" s="111"/>
+      <c r="F35" s="111"/>
+      <c r="G35" s="112"/>
       <c r="H35" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="I35" s="116"/>
+      <c r="I35" s="104"/>
       <c r="J35" s="62"/>
       <c r="K35" s="62"/>
       <c r="L35" s="69"/>
@@ -3359,17 +3146,17 @@
       <c r="B36" s="60">
         <v>6</v>
       </c>
-      <c r="C36" s="151" t="s">
+      <c r="C36" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="D36" s="152"/>
-      <c r="E36" s="152"/>
-      <c r="F36" s="152"/>
-      <c r="G36" s="153"/>
+      <c r="D36" s="111"/>
+      <c r="E36" s="111"/>
+      <c r="F36" s="111"/>
+      <c r="G36" s="112"/>
       <c r="H36" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="I36" s="116"/>
+      <c r="I36" s="104"/>
       <c r="J36" s="62"/>
       <c r="K36" s="62"/>
       <c r="L36" s="69"/>
@@ -3383,19 +3170,17 @@
       <c r="B37" s="64">
         <v>7</v>
       </c>
-      <c r="C37" s="151" t="s">
+      <c r="C37" s="110" t="s">
         <v>63</v>
       </c>
-      <c r="D37" s="152"/>
-      <c r="E37" s="152"/>
-      <c r="F37" s="152"/>
-      <c r="G37" s="153"/>
+      <c r="D37" s="111"/>
+      <c r="E37" s="111"/>
+      <c r="F37" s="111"/>
+      <c r="G37" s="112"/>
       <c r="H37" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="I37" s="117" t="s">
-        <v>73</v>
-      </c>
+      <c r="I37" s="105"/>
       <c r="J37" s="62"/>
       <c r="K37" s="62"/>
       <c r="L37" s="69"/>
@@ -3409,19 +3194,17 @@
       <c r="B38" s="64">
         <v>8</v>
       </c>
-      <c r="C38" s="151" t="s">
+      <c r="C38" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="D38" s="152"/>
-      <c r="E38" s="152"/>
-      <c r="F38" s="152"/>
-      <c r="G38" s="153"/>
+      <c r="D38" s="111"/>
+      <c r="E38" s="111"/>
+      <c r="F38" s="111"/>
+      <c r="G38" s="112"/>
       <c r="H38" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="I38" s="117" t="s">
-        <v>73</v>
-      </c>
+      <c r="I38" s="105"/>
       <c r="J38" s="62"/>
       <c r="K38" s="62"/>
       <c r="L38" s="69"/>
@@ -3435,19 +3218,17 @@
       <c r="B39" s="60">
         <v>9</v>
       </c>
-      <c r="C39" s="151" t="s">
+      <c r="C39" s="110" t="s">
         <v>65</v>
       </c>
-      <c r="D39" s="152"/>
-      <c r="E39" s="152"/>
-      <c r="F39" s="152"/>
-      <c r="G39" s="153"/>
+      <c r="D39" s="111"/>
+      <c r="E39" s="111"/>
+      <c r="F39" s="111"/>
+      <c r="G39" s="112"/>
       <c r="H39" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="I39" s="117" t="s">
-        <v>73</v>
-      </c>
+      <c r="I39" s="105"/>
       <c r="J39" s="62"/>
       <c r="K39" s="62"/>
       <c r="L39" s="69"/>
@@ -3473,31 +3254,31 @@
     </row>
     <row r="41" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="59"/>
-      <c r="B41" s="132" t="s">
+      <c r="B41" s="113" t="s">
         <v>48</v>
       </c>
-      <c r="C41" s="132"/>
-      <c r="D41" s="132"/>
-      <c r="E41" s="132"/>
-      <c r="F41" s="132"/>
+      <c r="C41" s="113"/>
+      <c r="D41" s="113"/>
+      <c r="E41" s="113"/>
+      <c r="F41" s="113"/>
       <c r="G41" s="77"/>
-      <c r="H41" s="121" t="s">
+      <c r="H41" s="134" t="s">
         <v>26</v>
       </c>
-      <c r="I41" s="122"/>
-      <c r="J41" s="155"/>
-      <c r="K41" s="155"/>
-      <c r="L41" s="122"/>
+      <c r="I41" s="108"/>
+      <c r="J41" s="107"/>
+      <c r="K41" s="107"/>
+      <c r="L41" s="108"/>
       <c r="M41" s="32"/>
       <c r="W41" s="66"/>
     </row>
     <row r="42" spans="1:23" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="59"/>
-      <c r="B42" s="133" t="s">
+      <c r="B42" s="144" t="s">
         <v>54</v>
       </c>
-      <c r="C42" s="133"/>
-      <c r="D42" s="133"/>
+      <c r="C42" s="144"/>
+      <c r="D42" s="144"/>
       <c r="E42" s="78" t="s">
         <v>53</v>
       </c>
@@ -3505,25 +3286,23 @@
         <v>68</v>
       </c>
       <c r="G42" s="77"/>
-      <c r="H42" s="131" t="s">
+      <c r="H42" s="143" t="s">
         <v>27</v>
       </c>
-      <c r="I42" s="131"/>
-      <c r="J42" s="130" t="s">
-        <v>85</v>
-      </c>
-      <c r="K42" s="130"/>
-      <c r="L42" s="130"/>
+      <c r="I42" s="143"/>
+      <c r="J42" s="142"/>
+      <c r="K42" s="142"/>
+      <c r="L42" s="142"/>
       <c r="M42" s="32"/>
       <c r="W42" s="66"/>
     </row>
     <row r="43" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="59"/>
-      <c r="B43" s="134" t="s">
+      <c r="B43" s="109" t="s">
         <v>57</v>
       </c>
-      <c r="C43" s="134"/>
-      <c r="D43" s="134"/>
+      <c r="C43" s="109"/>
+      <c r="D43" s="109"/>
       <c r="E43" s="79" t="s">
         <v>23</v>
       </c>
@@ -3531,25 +3310,23 @@
         <v>69</v>
       </c>
       <c r="G43" s="77"/>
-      <c r="H43" s="131" t="s">
+      <c r="H43" s="143" t="s">
         <v>28</v>
       </c>
-      <c r="I43" s="131"/>
-      <c r="J43" s="123" t="s">
-        <v>86</v>
-      </c>
-      <c r="K43" s="123"/>
-      <c r="L43" s="124"/>
+      <c r="I43" s="143"/>
+      <c r="J43" s="135"/>
+      <c r="K43" s="135"/>
+      <c r="L43" s="136"/>
       <c r="M43" s="32"/>
       <c r="W43" s="66"/>
     </row>
     <row r="44" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="59"/>
-      <c r="B44" s="134" t="s">
+      <c r="B44" s="109" t="s">
         <v>58</v>
       </c>
-      <c r="C44" s="134"/>
-      <c r="D44" s="134"/>
+      <c r="C44" s="109"/>
+      <c r="D44" s="109"/>
       <c r="E44" s="79" t="s">
         <v>22</v>
       </c>
@@ -3557,20 +3334,20 @@
         <v>69</v>
       </c>
       <c r="G44" s="77"/>
-      <c r="H44" s="131"/>
-      <c r="I44" s="131"/>
-      <c r="J44" s="125"/>
-      <c r="K44" s="125"/>
-      <c r="L44" s="126"/>
+      <c r="H44" s="143"/>
+      <c r="I44" s="143"/>
+      <c r="J44" s="137"/>
+      <c r="K44" s="137"/>
+      <c r="L44" s="138"/>
       <c r="M44" s="32"/>
     </row>
     <row r="45" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="59"/>
-      <c r="B45" s="156" t="s">
+      <c r="B45" s="114" t="s">
         <v>59</v>
       </c>
-      <c r="C45" s="156"/>
-      <c r="D45" s="156"/>
+      <c r="C45" s="114"/>
+      <c r="D45" s="114"/>
       <c r="E45" s="79" t="s">
         <v>21</v>
       </c>
@@ -3578,41 +3355,39 @@
         <v>69</v>
       </c>
       <c r="G45" s="77"/>
-      <c r="H45" s="131" t="s">
+      <c r="H45" s="143" t="s">
         <v>29</v>
       </c>
-      <c r="I45" s="131"/>
-      <c r="J45" s="123" t="s">
-        <v>87</v>
-      </c>
-      <c r="K45" s="123"/>
-      <c r="L45" s="124"/>
+      <c r="I45" s="143"/>
+      <c r="J45" s="135"/>
+      <c r="K45" s="135"/>
+      <c r="L45" s="136"/>
       <c r="M45" s="32"/>
     </row>
     <row r="46" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="59"/>
-      <c r="B46" s="132" t="s">
+      <c r="B46" s="113" t="s">
         <v>49</v>
       </c>
-      <c r="C46" s="132"/>
-      <c r="D46" s="132"/>
-      <c r="E46" s="132"/>
-      <c r="F46" s="132"/>
+      <c r="C46" s="113"/>
+      <c r="D46" s="113"/>
+      <c r="E46" s="113"/>
+      <c r="F46" s="113"/>
       <c r="G46" s="77"/>
-      <c r="H46" s="131"/>
-      <c r="I46" s="131"/>
-      <c r="J46" s="125"/>
-      <c r="K46" s="125"/>
-      <c r="L46" s="126"/>
+      <c r="H46" s="143"/>
+      <c r="I46" s="143"/>
+      <c r="J46" s="137"/>
+      <c r="K46" s="137"/>
+      <c r="L46" s="138"/>
       <c r="M46" s="32"/>
     </row>
     <row r="47" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="59"/>
-      <c r="B47" s="156" t="s">
+      <c r="B47" s="114" t="s">
         <v>60</v>
       </c>
-      <c r="C47" s="156"/>
-      <c r="D47" s="156"/>
+      <c r="C47" s="114"/>
+      <c r="D47" s="114"/>
       <c r="E47" s="79" t="s">
         <v>20</v>
       </c>
@@ -3620,20 +3395,20 @@
         <v>70</v>
       </c>
       <c r="G47" s="77"/>
-      <c r="H47" s="127"/>
-      <c r="I47" s="127"/>
-      <c r="J47" s="128"/>
-      <c r="K47" s="128"/>
-      <c r="L47" s="129"/>
+      <c r="H47" s="139"/>
+      <c r="I47" s="139"/>
+      <c r="J47" s="140"/>
+      <c r="K47" s="140"/>
+      <c r="L47" s="141"/>
       <c r="M47" s="32"/>
     </row>
     <row r="48" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="59"/>
-      <c r="B48" s="134" t="s">
+      <c r="B48" s="109" t="s">
         <v>55</v>
       </c>
-      <c r="C48" s="134"/>
-      <c r="D48" s="134"/>
+      <c r="C48" s="109"/>
+      <c r="D48" s="109"/>
       <c r="E48" s="79" t="s">
         <v>21</v>
       </c>
@@ -3641,20 +3416,20 @@
         <v>70</v>
       </c>
       <c r="G48" s="77"/>
-      <c r="H48" s="127"/>
-      <c r="I48" s="127"/>
-      <c r="J48" s="128"/>
-      <c r="K48" s="128"/>
-      <c r="L48" s="129"/>
+      <c r="H48" s="139"/>
+      <c r="I48" s="139"/>
+      <c r="J48" s="140"/>
+      <c r="K48" s="140"/>
+      <c r="L48" s="141"/>
       <c r="M48" s="32"/>
     </row>
     <row r="49" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="59"/>
-      <c r="B49" s="134" t="s">
+      <c r="B49" s="109" t="s">
         <v>56</v>
       </c>
-      <c r="C49" s="134"/>
-      <c r="D49" s="134"/>
+      <c r="C49" s="109"/>
+      <c r="D49" s="109"/>
       <c r="E49" s="79" t="s">
         <v>21</v>
       </c>
@@ -3772,15 +3547,15 @@
       <c r="M56" s="32"/>
     </row>
     <row r="57" spans="1:13" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="120"/>
-      <c r="C57" s="120"/>
-      <c r="D57" s="120"/>
-      <c r="E57" s="120"/>
-      <c r="F57" s="120"/>
-      <c r="G57" s="120"/>
-      <c r="H57" s="120"/>
-      <c r="I57" s="120"/>
-      <c r="J57" s="120"/>
+      <c r="B57" s="133"/>
+      <c r="C57" s="133"/>
+      <c r="D57" s="133"/>
+      <c r="E57" s="133"/>
+      <c r="F57" s="133"/>
+      <c r="G57" s="133"/>
+      <c r="H57" s="133"/>
+      <c r="I57" s="133"/>
+      <c r="J57" s="133"/>
       <c r="K57" s="29"/>
       <c r="L57" s="66"/>
       <c r="M57" s="32"/>
@@ -3823,20 +3598,20 @@
     </row>
     <row r="60" spans="1:13" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="61" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="119" t="s">
-        <v>74</v>
-      </c>
-      <c r="B61" s="119"/>
-      <c r="C61" s="119"/>
-      <c r="D61" s="119"/>
-      <c r="E61" s="119"/>
-      <c r="F61" s="119"/>
-      <c r="G61" s="119"/>
-      <c r="H61" s="119"/>
-      <c r="I61" s="119"/>
-      <c r="J61" s="119"/>
-      <c r="K61" s="119"/>
-      <c r="L61" s="119"/>
+      <c r="A61" s="132" t="s">
+        <v>73</v>
+      </c>
+      <c r="B61" s="132"/>
+      <c r="C61" s="132"/>
+      <c r="D61" s="132"/>
+      <c r="E61" s="132"/>
+      <c r="F61" s="132"/>
+      <c r="G61" s="132"/>
+      <c r="H61" s="132"/>
+      <c r="I61" s="132"/>
+      <c r="J61" s="132"/>
+      <c r="K61" s="132"/>
+      <c r="L61" s="132"/>
     </row>
     <row r="62" spans="1:13" ht="15.9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="63" spans="1:13" ht="15.9" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3846,6 +3621,39 @@
     <protectedRange sqref="C57" name="Rango3_3_1_1_1_1_1_2_1"/>
   </protectedRanges>
   <mergeCells count="49">
+    <mergeCell ref="A61:L61"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="E57:H57"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="J43:L44"/>
+    <mergeCell ref="J45:L46"/>
+    <mergeCell ref="H47:I48"/>
+    <mergeCell ref="J47:L48"/>
+    <mergeCell ref="J42:L42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="H45:I46"/>
+    <mergeCell ref="H43:I44"/>
+    <mergeCell ref="A7:L7"/>
+    <mergeCell ref="A8:L8"/>
+    <mergeCell ref="A14:L14"/>
+    <mergeCell ref="A17:I17"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="H25:J25"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="A15:L15"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
     <mergeCell ref="J41:L41"/>
     <mergeCell ref="B48:D48"/>
     <mergeCell ref="C31:G31"/>
@@ -3862,39 +3670,6 @@
     <mergeCell ref="C36:G36"/>
     <mergeCell ref="C37:G37"/>
     <mergeCell ref="C38:G38"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="H25:J25"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="A15:L15"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="A7:L7"/>
-    <mergeCell ref="A8:L8"/>
-    <mergeCell ref="A14:L14"/>
-    <mergeCell ref="A17:I17"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A61:L61"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="E57:H57"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="J43:L44"/>
-    <mergeCell ref="J45:L46"/>
-    <mergeCell ref="H47:I48"/>
-    <mergeCell ref="J47:L48"/>
-    <mergeCell ref="J42:L42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="H45:I46"/>
-    <mergeCell ref="H43:I44"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="A18:A22">
@@ -3903,12 +3678,7 @@
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q18">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="no">
-      <formula>NOT(ISERROR(SEARCH("no",Q18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="5">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J18:J21" xr:uid="{5880DEF5-77FD-4C64-B181-2DF87D702053}">
       <formula1>"-, NO, SI"</formula1>
     </dataValidation>
@@ -3920,9 +3690,6 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J45:L46" xr:uid="{0D6AB881-FC6E-4596-A1C9-58E066442A98}">
       <formula1>"-, EQP-0049"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P16" xr:uid="{535E85A9-1FDF-4340-9879-4F3781F64439}">
-      <formula1>$N$22:$N$32</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -3954,10 +3721,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="157" t="s">
+      <c r="A2" s="145" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="157"/>
+      <c r="B2" s="145"/>
       <c r="C2" s="5" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
feat(recepcion): mejorar extracción excel y actualizar template humedad
</commit_message>
<xml_diff>
--- a/app/templates/Template_Humedad.xlsx
+++ b/app/templates/Template_Humedad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\crmnew\api-geofal-crm\app\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40ABFF1-F9A4-4FE4-BAFB-15FF1B5D5AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBCBA63-BEB9-492D-B25C-C4005850A48B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="723" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="78">
   <si>
     <t>FC</t>
   </si>
@@ -257,6 +257,18 @@
   </si>
   <si>
     <t>WEB: www.geofal.com.pe   E-MAIL: laboratorio@geofal.com.pe                                                                                                                                                                         Av. Marañon 763, Los Olivos-Lima / Teléfono  01 754-3070</t>
+  </si>
+  <si>
+    <t>MUESTRA</t>
+  </si>
+  <si>
+    <t>N° OT</t>
+  </si>
+  <si>
+    <t>FECHA DE ENSAYO</t>
+  </si>
+  <si>
+    <t>REALIZADO</t>
   </si>
 </sst>
 </file>
@@ -269,7 +281,7 @@
     <numFmt numFmtId="166" formatCode="0\ &quot;/ CO-06&quot;"/>
     <numFmt numFmtId="167" formatCode="&quot;FORMATO F-LEM-P-SU-11.01&quot;"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -395,6 +407,12 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -658,7 +676,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -998,95 +1016,6 @@
     <xf numFmtId="1" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="16" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1094,6 +1023,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -1134,11 +1067,102 @@
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1287,580 +1311,6 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>205560</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="5 CuadroTexto">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="200025" y="1379220"/>
-          <a:ext cx="1560015" cy="255270"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-PE" sz="900">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>MUESTRA</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>253365</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="6 CuadroTexto">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1807845" y="1379220"/>
-          <a:ext cx="1569720" cy="255270"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-PE" sz="900">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>N°</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-PE" sz="900" baseline="0">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> OT</a:t>
-          </a:r>
-          <a:endParaRPr lang="es-PE" sz="900">
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>160020</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>146505</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="8 CuadroTexto">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3451860" y="1379220"/>
-          <a:ext cx="1609545" cy="255270"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-PE" sz="900">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>FECHA DE</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-PE" sz="900" baseline="0">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> ENSAYO</a:t>
-          </a:r>
-          <a:endParaRPr lang="es-PE" sz="900">
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>87630</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>205560</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="4 Rectángulo">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="200025" y="1664970"/>
-          <a:ext cx="1560015" cy="308610"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="3175">
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="es-PE" sz="900">
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="4 Rectángulo">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1821180" y="1672590"/>
-          <a:ext cx="1556385" cy="300990"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="3175">
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="es-PE" sz="900">
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>160020</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>146505</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="4 Rectángulo">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3451860" y="1682115"/>
-          <a:ext cx="1609545" cy="300990"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="3175">
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="es-PE" sz="900">
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>180974</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>447674</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="19" name="6 CuadroTexto">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45F78A96-B9D0-4DA3-835F-CFBB406A79D7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5095874" y="1379220"/>
-          <a:ext cx="2095500" cy="255270"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-PE" sz="900">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>REALIZADO</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>194309</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>445760</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="20" name="4 Rectángulo">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBC2EA0B-0992-45F5-AE2F-86236C249B06}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5109209" y="1672590"/>
-          <a:ext cx="2080251" cy="300990"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="3175">
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="es-PE" sz="900">
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
@@ -2114,6 +1564,258 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>251460</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>526732</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>16193</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectángulo 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3450E0D-4F26-4E52-9FCC-E3A986384AD2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3543300" y="1371600"/>
+          <a:ext cx="1258252" cy="221933"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="12700">
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-PE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>992777</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>16193</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectángulo 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{443FDFFB-FF16-49CE-8274-3A3549CBB661}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5069477" y="1380309"/>
+          <a:ext cx="847997" cy="225198"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="12700">
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-PE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>622663</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>8709</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>721723</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>33610</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rectángulo 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{325CB4C3-5063-4F15-B269-4F3E096A533B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1432560" y="1397726"/>
+          <a:ext cx="847997" cy="225198"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="12700">
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-PE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>971007</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>77289</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Rectángulo 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5F863DF-5F5E-4CAF-97F2-E3D55EF4B1DB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2529841" y="1389017"/>
+          <a:ext cx="847997" cy="230777"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="12700">
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-PE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2549,8 +2251,8 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:W63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14:Q32"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="175" zoomScaleNormal="100" zoomScaleSheetLayoutView="175" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.33203125" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2652,36 +2354,36 @@
       <c r="L6" s="26"/>
     </row>
     <row r="7" spans="1:13" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="125" t="s">
+      <c r="A7" s="123" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="125"/>
-      <c r="C7" s="125"/>
-      <c r="D7" s="125"/>
-      <c r="E7" s="125"/>
-      <c r="F7" s="125"/>
-      <c r="G7" s="125"/>
-      <c r="H7" s="125"/>
-      <c r="I7" s="125"/>
-      <c r="J7" s="125"/>
-      <c r="K7" s="125"/>
-      <c r="L7" s="125"/>
+      <c r="B7" s="123"/>
+      <c r="C7" s="123"/>
+      <c r="D7" s="123"/>
+      <c r="E7" s="123"/>
+      <c r="F7" s="123"/>
+      <c r="G7" s="123"/>
+      <c r="H7" s="123"/>
+      <c r="I7" s="123"/>
+      <c r="J7" s="123"/>
+      <c r="K7" s="123"/>
+      <c r="L7" s="123"/>
     </row>
     <row r="8" spans="1:13" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="126" t="s">
+      <c r="A8" s="124" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="126"/>
-      <c r="C8" s="126"/>
-      <c r="D8" s="126"/>
-      <c r="E8" s="126"/>
-      <c r="F8" s="126"/>
-      <c r="G8" s="126"/>
-      <c r="H8" s="126"/>
-      <c r="I8" s="126"/>
-      <c r="J8" s="126"/>
-      <c r="K8" s="126"/>
-      <c r="L8" s="126"/>
+      <c r="B8" s="124"/>
+      <c r="C8" s="124"/>
+      <c r="D8" s="124"/>
+      <c r="E8" s="124"/>
+      <c r="F8" s="124"/>
+      <c r="G8" s="124"/>
+      <c r="H8" s="124"/>
+      <c r="I8" s="124"/>
+      <c r="J8" s="124"/>
+      <c r="K8" s="124"/>
+      <c r="L8" s="124"/>
     </row>
     <row r="9" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27"/>
@@ -2700,13 +2402,20 @@
     <row r="10" spans="1:13" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="27"/>
       <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
+      <c r="D10" s="147" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="146" t="s">
+        <v>75</v>
+      </c>
       <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
+      <c r="G10" s="146" t="s">
+        <v>76</v>
+      </c>
       <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
+      <c r="I10" s="146" t="s">
+        <v>77</v>
+      </c>
       <c r="J10" s="27"/>
       <c r="K10" s="27"/>
       <c r="L10" s="27"/>
@@ -2729,12 +2438,12 @@
       <c r="A12" s="27"/>
       <c r="B12" s="27"/>
       <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
       <c r="J12" s="27"/>
       <c r="K12" s="27"/>
       <c r="L12" s="27"/>
@@ -2755,37 +2464,37 @@
       <c r="M13" s="32"/>
     </row>
     <row r="14" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="127" t="s">
+      <c r="A14" s="125" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="128"/>
-      <c r="C14" s="128"/>
-      <c r="D14" s="128"/>
-      <c r="E14" s="128"/>
-      <c r="F14" s="128"/>
-      <c r="G14" s="128"/>
-      <c r="H14" s="128"/>
-      <c r="I14" s="128"/>
-      <c r="J14" s="128"/>
-      <c r="K14" s="128"/>
-      <c r="L14" s="129"/>
+      <c r="B14" s="126"/>
+      <c r="C14" s="126"/>
+      <c r="D14" s="126"/>
+      <c r="E14" s="126"/>
+      <c r="F14" s="126"/>
+      <c r="G14" s="126"/>
+      <c r="H14" s="126"/>
+      <c r="I14" s="126"/>
+      <c r="J14" s="126"/>
+      <c r="K14" s="126"/>
+      <c r="L14" s="127"/>
       <c r="M14" s="32"/>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="119" t="s">
+      <c r="A15" s="134" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="120"/>
-      <c r="C15" s="120"/>
-      <c r="D15" s="120"/>
-      <c r="E15" s="120"/>
-      <c r="F15" s="120"/>
-      <c r="G15" s="120"/>
-      <c r="H15" s="120"/>
-      <c r="I15" s="120"/>
-      <c r="J15" s="120"/>
-      <c r="K15" s="120"/>
-      <c r="L15" s="121"/>
+      <c r="B15" s="135"/>
+      <c r="C15" s="135"/>
+      <c r="D15" s="135"/>
+      <c r="E15" s="135"/>
+      <c r="F15" s="135"/>
+      <c r="G15" s="135"/>
+      <c r="H15" s="135"/>
+      <c r="I15" s="135"/>
+      <c r="J15" s="135"/>
+      <c r="K15" s="135"/>
+      <c r="L15" s="136"/>
       <c r="M15" s="32"/>
     </row>
     <row r="16" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2804,17 +2513,17 @@
       <c r="M16" s="32"/>
     </row>
     <row r="17" spans="1:19" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="130" t="s">
+      <c r="A17" s="128" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="131"/>
-      <c r="C17" s="131"/>
-      <c r="D17" s="131"/>
-      <c r="E17" s="131"/>
-      <c r="F17" s="131"/>
-      <c r="G17" s="131"/>
-      <c r="H17" s="131"/>
-      <c r="I17" s="131"/>
+      <c r="B17" s="129"/>
+      <c r="C17" s="129"/>
+      <c r="D17" s="129"/>
+      <c r="E17" s="129"/>
+      <c r="F17" s="129"/>
+      <c r="G17" s="129"/>
+      <c r="H17" s="129"/>
+      <c r="I17" s="129"/>
       <c r="J17" s="37"/>
       <c r="K17" s="37"/>
       <c r="L17" s="38"/>
@@ -2914,12 +2623,12 @@
       <c r="L23" s="38"/>
     </row>
     <row r="24" spans="1:19" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="130" t="s">
+      <c r="A24" s="128" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="131"/>
-      <c r="C24" s="131"/>
-      <c r="D24" s="131"/>
+      <c r="B24" s="129"/>
+      <c r="C24" s="129"/>
+      <c r="D24" s="129"/>
       <c r="E24" s="43"/>
       <c r="F24" s="43"/>
       <c r="G24" s="43"/>
@@ -2930,55 +2639,55 @@
       <c r="L24" s="38"/>
     </row>
     <row r="25" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="123" t="s">
+      <c r="A25" s="138" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="123"/>
-      <c r="C25" s="123"/>
-      <c r="D25" s="123"/>
-      <c r="E25" s="124"/>
-      <c r="F25" s="124"/>
+      <c r="B25" s="138"/>
+      <c r="C25" s="138"/>
+      <c r="D25" s="138"/>
+      <c r="E25" s="139"/>
+      <c r="F25" s="139"/>
       <c r="G25" s="44"/>
-      <c r="H25" s="116" t="s">
+      <c r="H25" s="131" t="s">
         <v>42</v>
       </c>
-      <c r="I25" s="117"/>
-      <c r="J25" s="118"/>
+      <c r="I25" s="132"/>
+      <c r="J25" s="133"/>
       <c r="K25" s="45"/>
       <c r="L25" s="38"/>
     </row>
     <row r="26" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="123" t="s">
+      <c r="A26" s="138" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="123"/>
-      <c r="C26" s="123"/>
-      <c r="D26" s="123"/>
-      <c r="E26" s="124"/>
-      <c r="F26" s="124"/>
+      <c r="B26" s="138"/>
+      <c r="C26" s="138"/>
+      <c r="D26" s="138"/>
+      <c r="E26" s="139"/>
+      <c r="F26" s="139"/>
       <c r="G26" s="44"/>
-      <c r="H26" s="116" t="s">
+      <c r="H26" s="131" t="s">
         <v>31</v>
       </c>
-      <c r="I26" s="118"/>
+      <c r="I26" s="133"/>
       <c r="J26" s="103"/>
       <c r="K26" s="46"/>
       <c r="L26" s="38"/>
     </row>
     <row r="27" spans="1:19" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="123" t="s">
+      <c r="A27" s="138" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="123"/>
-      <c r="C27" s="123"/>
-      <c r="D27" s="123"/>
-      <c r="E27" s="124"/>
-      <c r="F27" s="124"/>
+      <c r="B27" s="138"/>
+      <c r="C27" s="138"/>
+      <c r="D27" s="138"/>
+      <c r="E27" s="139"/>
+      <c r="F27" s="139"/>
       <c r="G27" s="44"/>
-      <c r="H27" s="116" t="s">
+      <c r="H27" s="131" t="s">
         <v>32</v>
       </c>
-      <c r="I27" s="118"/>
+      <c r="I27" s="133"/>
       <c r="J27" s="103"/>
       <c r="K27" s="46"/>
       <c r="L27" s="38"/>
@@ -3009,22 +2718,22 @@
     </row>
     <row r="30" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="56"/>
-      <c r="B30" s="115" t="s">
+      <c r="B30" s="130" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="115"/>
-      <c r="D30" s="115"/>
-      <c r="E30" s="115"/>
-      <c r="F30" s="115"/>
-      <c r="G30" s="115"/>
+      <c r="C30" s="130"/>
+      <c r="D30" s="130"/>
+      <c r="E30" s="130"/>
+      <c r="F30" s="130"/>
+      <c r="G30" s="130"/>
       <c r="H30" s="57" t="s">
         <v>44</v>
       </c>
       <c r="I30" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="J30" s="122"/>
-      <c r="K30" s="122"/>
+      <c r="J30" s="137"/>
+      <c r="K30" s="137"/>
       <c r="L30" s="58"/>
       <c r="M30" s="32"/>
     </row>
@@ -3033,13 +2742,13 @@
       <c r="B31" s="60">
         <v>1</v>
       </c>
-      <c r="C31" s="110" t="s">
+      <c r="C31" s="141" t="s">
         <v>17</v>
       </c>
-      <c r="D31" s="111"/>
-      <c r="E31" s="111"/>
-      <c r="F31" s="111"/>
-      <c r="G31" s="112"/>
+      <c r="D31" s="142"/>
+      <c r="E31" s="142"/>
+      <c r="F31" s="142"/>
+      <c r="G31" s="143"/>
       <c r="H31" s="61" t="s">
         <v>18</v>
       </c>
@@ -3054,13 +2763,13 @@
       <c r="B32" s="64">
         <v>2</v>
       </c>
-      <c r="C32" s="110" t="s">
+      <c r="C32" s="141" t="s">
         <v>39</v>
       </c>
-      <c r="D32" s="111"/>
-      <c r="E32" s="111"/>
-      <c r="F32" s="111"/>
-      <c r="G32" s="112"/>
+      <c r="D32" s="142"/>
+      <c r="E32" s="142"/>
+      <c r="F32" s="142"/>
+      <c r="G32" s="143"/>
       <c r="H32" s="61" t="s">
         <v>18</v>
       </c>
@@ -3076,13 +2785,13 @@
       <c r="B33" s="64">
         <v>3</v>
       </c>
-      <c r="C33" s="110" t="s">
+      <c r="C33" s="141" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="111"/>
-      <c r="E33" s="111"/>
-      <c r="F33" s="111"/>
-      <c r="G33" s="112"/>
+      <c r="D33" s="142"/>
+      <c r="E33" s="142"/>
+      <c r="F33" s="142"/>
+      <c r="G33" s="143"/>
       <c r="H33" s="61" t="s">
         <v>33</v>
       </c>
@@ -3098,13 +2807,13 @@
       <c r="B34" s="60">
         <v>4</v>
       </c>
-      <c r="C34" s="110" t="s">
+      <c r="C34" s="141" t="s">
         <v>61</v>
       </c>
-      <c r="D34" s="111"/>
-      <c r="E34" s="111"/>
-      <c r="F34" s="111"/>
-      <c r="G34" s="112"/>
+      <c r="D34" s="142"/>
+      <c r="E34" s="142"/>
+      <c r="F34" s="142"/>
+      <c r="G34" s="143"/>
       <c r="H34" s="61" t="s">
         <v>33</v>
       </c>
@@ -3122,13 +2831,13 @@
       <c r="B35" s="64">
         <v>5</v>
       </c>
-      <c r="C35" s="110" t="s">
+      <c r="C35" s="141" t="s">
         <v>62</v>
       </c>
-      <c r="D35" s="111"/>
-      <c r="E35" s="111"/>
-      <c r="F35" s="111"/>
-      <c r="G35" s="112"/>
+      <c r="D35" s="142"/>
+      <c r="E35" s="142"/>
+      <c r="F35" s="142"/>
+      <c r="G35" s="143"/>
       <c r="H35" s="61" t="s">
         <v>33</v>
       </c>
@@ -3146,13 +2855,13 @@
       <c r="B36" s="60">
         <v>6</v>
       </c>
-      <c r="C36" s="110" t="s">
+      <c r="C36" s="141" t="s">
         <v>41</v>
       </c>
-      <c r="D36" s="111"/>
-      <c r="E36" s="111"/>
-      <c r="F36" s="111"/>
-      <c r="G36" s="112"/>
+      <c r="D36" s="142"/>
+      <c r="E36" s="142"/>
+      <c r="F36" s="142"/>
+      <c r="G36" s="143"/>
       <c r="H36" s="61" t="s">
         <v>33</v>
       </c>
@@ -3170,13 +2879,13 @@
       <c r="B37" s="64">
         <v>7</v>
       </c>
-      <c r="C37" s="110" t="s">
+      <c r="C37" s="141" t="s">
         <v>63</v>
       </c>
-      <c r="D37" s="111"/>
-      <c r="E37" s="111"/>
-      <c r="F37" s="111"/>
-      <c r="G37" s="112"/>
+      <c r="D37" s="142"/>
+      <c r="E37" s="142"/>
+      <c r="F37" s="142"/>
+      <c r="G37" s="143"/>
       <c r="H37" s="61" t="s">
         <v>33</v>
       </c>
@@ -3194,13 +2903,13 @@
       <c r="B38" s="64">
         <v>8</v>
       </c>
-      <c r="C38" s="110" t="s">
+      <c r="C38" s="141" t="s">
         <v>64</v>
       </c>
-      <c r="D38" s="111"/>
-      <c r="E38" s="111"/>
-      <c r="F38" s="111"/>
-      <c r="G38" s="112"/>
+      <c r="D38" s="142"/>
+      <c r="E38" s="142"/>
+      <c r="F38" s="142"/>
+      <c r="G38" s="143"/>
       <c r="H38" s="61" t="s">
         <v>33</v>
       </c>
@@ -3218,13 +2927,13 @@
       <c r="B39" s="60">
         <v>9</v>
       </c>
-      <c r="C39" s="110" t="s">
+      <c r="C39" s="141" t="s">
         <v>65</v>
       </c>
-      <c r="D39" s="111"/>
-      <c r="E39" s="111"/>
-      <c r="F39" s="111"/>
-      <c r="G39" s="112"/>
+      <c r="D39" s="142"/>
+      <c r="E39" s="142"/>
+      <c r="F39" s="142"/>
+      <c r="G39" s="143"/>
       <c r="H39" s="61" t="s">
         <v>19</v>
       </c>
@@ -3254,31 +2963,31 @@
     </row>
     <row r="41" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="59"/>
-      <c r="B41" s="113" t="s">
+      <c r="B41" s="120" t="s">
         <v>48</v>
       </c>
-      <c r="C41" s="113"/>
-      <c r="D41" s="113"/>
-      <c r="E41" s="113"/>
-      <c r="F41" s="113"/>
+      <c r="C41" s="120"/>
+      <c r="D41" s="120"/>
+      <c r="E41" s="120"/>
+      <c r="F41" s="120"/>
       <c r="G41" s="77"/>
-      <c r="H41" s="134" t="s">
+      <c r="H41" s="109" t="s">
         <v>26</v>
       </c>
-      <c r="I41" s="108"/>
-      <c r="J41" s="107"/>
-      <c r="K41" s="107"/>
-      <c r="L41" s="108"/>
+      <c r="I41" s="110"/>
+      <c r="J41" s="140"/>
+      <c r="K41" s="140"/>
+      <c r="L41" s="110"/>
       <c r="M41" s="32"/>
       <c r="W41" s="66"/>
     </row>
     <row r="42" spans="1:23" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="59"/>
-      <c r="B42" s="144" t="s">
+      <c r="B42" s="121" t="s">
         <v>54</v>
       </c>
-      <c r="C42" s="144"/>
-      <c r="D42" s="144"/>
+      <c r="C42" s="121"/>
+      <c r="D42" s="121"/>
       <c r="E42" s="78" t="s">
         <v>53</v>
       </c>
@@ -3286,23 +2995,23 @@
         <v>68</v>
       </c>
       <c r="G42" s="77"/>
-      <c r="H42" s="143" t="s">
+      <c r="H42" s="119" t="s">
         <v>27</v>
       </c>
-      <c r="I42" s="143"/>
-      <c r="J42" s="142"/>
-      <c r="K42" s="142"/>
-      <c r="L42" s="142"/>
+      <c r="I42" s="119"/>
+      <c r="J42" s="118"/>
+      <c r="K42" s="118"/>
+      <c r="L42" s="118"/>
       <c r="M42" s="32"/>
       <c r="W42" s="66"/>
     </row>
     <row r="43" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="59"/>
-      <c r="B43" s="109" t="s">
+      <c r="B43" s="122" t="s">
         <v>57</v>
       </c>
-      <c r="C43" s="109"/>
-      <c r="D43" s="109"/>
+      <c r="C43" s="122"/>
+      <c r="D43" s="122"/>
       <c r="E43" s="79" t="s">
         <v>23</v>
       </c>
@@ -3310,23 +3019,23 @@
         <v>69</v>
       </c>
       <c r="G43" s="77"/>
-      <c r="H43" s="143" t="s">
+      <c r="H43" s="119" t="s">
         <v>28</v>
       </c>
-      <c r="I43" s="143"/>
-      <c r="J43" s="135"/>
-      <c r="K43" s="135"/>
-      <c r="L43" s="136"/>
+      <c r="I43" s="119"/>
+      <c r="J43" s="111"/>
+      <c r="K43" s="111"/>
+      <c r="L43" s="112"/>
       <c r="M43" s="32"/>
       <c r="W43" s="66"/>
     </row>
     <row r="44" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="59"/>
-      <c r="B44" s="109" t="s">
+      <c r="B44" s="122" t="s">
         <v>58</v>
       </c>
-      <c r="C44" s="109"/>
-      <c r="D44" s="109"/>
+      <c r="C44" s="122"/>
+      <c r="D44" s="122"/>
       <c r="E44" s="79" t="s">
         <v>22</v>
       </c>
@@ -3334,20 +3043,20 @@
         <v>69</v>
       </c>
       <c r="G44" s="77"/>
-      <c r="H44" s="143"/>
-      <c r="I44" s="143"/>
-      <c r="J44" s="137"/>
-      <c r="K44" s="137"/>
-      <c r="L44" s="138"/>
+      <c r="H44" s="119"/>
+      <c r="I44" s="119"/>
+      <c r="J44" s="113"/>
+      <c r="K44" s="113"/>
+      <c r="L44" s="114"/>
       <c r="M44" s="32"/>
     </row>
     <row r="45" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="59"/>
-      <c r="B45" s="114" t="s">
+      <c r="B45" s="144" t="s">
         <v>59</v>
       </c>
-      <c r="C45" s="114"/>
-      <c r="D45" s="114"/>
+      <c r="C45" s="144"/>
+      <c r="D45" s="144"/>
       <c r="E45" s="79" t="s">
         <v>21</v>
       </c>
@@ -3355,39 +3064,39 @@
         <v>69</v>
       </c>
       <c r="G45" s="77"/>
-      <c r="H45" s="143" t="s">
+      <c r="H45" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="I45" s="143"/>
-      <c r="J45" s="135"/>
-      <c r="K45" s="135"/>
-      <c r="L45" s="136"/>
+      <c r="I45" s="119"/>
+      <c r="J45" s="111"/>
+      <c r="K45" s="111"/>
+      <c r="L45" s="112"/>
       <c r="M45" s="32"/>
     </row>
     <row r="46" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="59"/>
-      <c r="B46" s="113" t="s">
+      <c r="B46" s="120" t="s">
         <v>49</v>
       </c>
-      <c r="C46" s="113"/>
-      <c r="D46" s="113"/>
-      <c r="E46" s="113"/>
-      <c r="F46" s="113"/>
+      <c r="C46" s="120"/>
+      <c r="D46" s="120"/>
+      <c r="E46" s="120"/>
+      <c r="F46" s="120"/>
       <c r="G46" s="77"/>
-      <c r="H46" s="143"/>
-      <c r="I46" s="143"/>
-      <c r="J46" s="137"/>
-      <c r="K46" s="137"/>
-      <c r="L46" s="138"/>
+      <c r="H46" s="119"/>
+      <c r="I46" s="119"/>
+      <c r="J46" s="113"/>
+      <c r="K46" s="113"/>
+      <c r="L46" s="114"/>
       <c r="M46" s="32"/>
     </row>
     <row r="47" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="59"/>
-      <c r="B47" s="114" t="s">
+      <c r="B47" s="144" t="s">
         <v>60</v>
       </c>
-      <c r="C47" s="114"/>
-      <c r="D47" s="114"/>
+      <c r="C47" s="144"/>
+      <c r="D47" s="144"/>
       <c r="E47" s="79" t="s">
         <v>20</v>
       </c>
@@ -3395,20 +3104,20 @@
         <v>70</v>
       </c>
       <c r="G47" s="77"/>
-      <c r="H47" s="139"/>
-      <c r="I47" s="139"/>
-      <c r="J47" s="140"/>
-      <c r="K47" s="140"/>
-      <c r="L47" s="141"/>
+      <c r="H47" s="115"/>
+      <c r="I47" s="115"/>
+      <c r="J47" s="116"/>
+      <c r="K47" s="116"/>
+      <c r="L47" s="117"/>
       <c r="M47" s="32"/>
     </row>
     <row r="48" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="59"/>
-      <c r="B48" s="109" t="s">
+      <c r="B48" s="122" t="s">
         <v>55</v>
       </c>
-      <c r="C48" s="109"/>
-      <c r="D48" s="109"/>
+      <c r="C48" s="122"/>
+      <c r="D48" s="122"/>
       <c r="E48" s="79" t="s">
         <v>21</v>
       </c>
@@ -3416,20 +3125,20 @@
         <v>70</v>
       </c>
       <c r="G48" s="77"/>
-      <c r="H48" s="139"/>
-      <c r="I48" s="139"/>
-      <c r="J48" s="140"/>
-      <c r="K48" s="140"/>
-      <c r="L48" s="141"/>
+      <c r="H48" s="115"/>
+      <c r="I48" s="115"/>
+      <c r="J48" s="116"/>
+      <c r="K48" s="116"/>
+      <c r="L48" s="117"/>
       <c r="M48" s="32"/>
     </row>
     <row r="49" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="59"/>
-      <c r="B49" s="109" t="s">
+      <c r="B49" s="122" t="s">
         <v>56</v>
       </c>
-      <c r="C49" s="109"/>
-      <c r="D49" s="109"/>
+      <c r="C49" s="122"/>
+      <c r="D49" s="122"/>
       <c r="E49" s="79" t="s">
         <v>21</v>
       </c>
@@ -3547,15 +3256,15 @@
       <c r="M56" s="32"/>
     </row>
     <row r="57" spans="1:13" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="133"/>
-      <c r="C57" s="133"/>
-      <c r="D57" s="133"/>
-      <c r="E57" s="133"/>
-      <c r="F57" s="133"/>
-      <c r="G57" s="133"/>
-      <c r="H57" s="133"/>
-      <c r="I57" s="133"/>
-      <c r="J57" s="133"/>
+      <c r="B57" s="108"/>
+      <c r="C57" s="108"/>
+      <c r="D57" s="108"/>
+      <c r="E57" s="108"/>
+      <c r="F57" s="108"/>
+      <c r="G57" s="108"/>
+      <c r="H57" s="108"/>
+      <c r="I57" s="108"/>
+      <c r="J57" s="108"/>
       <c r="K57" s="29"/>
       <c r="L57" s="66"/>
       <c r="M57" s="32"/>
@@ -3598,20 +3307,20 @@
     </row>
     <row r="60" spans="1:13" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="61" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="132" t="s">
+      <c r="A61" s="107" t="s">
         <v>73</v>
       </c>
-      <c r="B61" s="132"/>
-      <c r="C61" s="132"/>
-      <c r="D61" s="132"/>
-      <c r="E61" s="132"/>
-      <c r="F61" s="132"/>
-      <c r="G61" s="132"/>
-      <c r="H61" s="132"/>
-      <c r="I61" s="132"/>
-      <c r="J61" s="132"/>
-      <c r="K61" s="132"/>
-      <c r="L61" s="132"/>
+      <c r="B61" s="107"/>
+      <c r="C61" s="107"/>
+      <c r="D61" s="107"/>
+      <c r="E61" s="107"/>
+      <c r="F61" s="107"/>
+      <c r="G61" s="107"/>
+      <c r="H61" s="107"/>
+      <c r="I61" s="107"/>
+      <c r="J61" s="107"/>
+      <c r="K61" s="107"/>
+      <c r="L61" s="107"/>
     </row>
     <row r="62" spans="1:13" ht="15.9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="63" spans="1:13" ht="15.9" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3621,6 +3330,39 @@
     <protectedRange sqref="C57" name="Rango3_3_1_1_1_1_1_2_1"/>
   </protectedRanges>
   <mergeCells count="49">
+    <mergeCell ref="J41:L41"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="H25:J25"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="A15:L15"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="A7:L7"/>
+    <mergeCell ref="A8:L8"/>
+    <mergeCell ref="A14:L14"/>
+    <mergeCell ref="A17:I17"/>
+    <mergeCell ref="A24:D24"/>
     <mergeCell ref="A61:L61"/>
     <mergeCell ref="B57:D57"/>
     <mergeCell ref="E57:H57"/>
@@ -3637,39 +3379,6 @@
     <mergeCell ref="B49:D49"/>
     <mergeCell ref="H45:I46"/>
     <mergeCell ref="H43:I44"/>
-    <mergeCell ref="A7:L7"/>
-    <mergeCell ref="A8:L8"/>
-    <mergeCell ref="A14:L14"/>
-    <mergeCell ref="A17:I17"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="H25:J25"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="A15:L15"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="J41:L41"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C39:G39"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C38:G38"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="A18:A22">

</xml_diff>

<commit_message>
feat: adaptar plantilla y exportacion humedad al nuevo formato
</commit_message>
<xml_diff>
--- a/app/templates/Template_Humedad.xlsx
+++ b/app/templates/Template_Humedad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\crmnew\api-geofal-crm\app\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBCBA63-BEB9-492D-B25C-C4005850A48B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{26ACD2A0-3DEE-4F31-BBF6-A5144280BE4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="723" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="81">
   <si>
     <t>FC</t>
   </si>
@@ -130,15 +130,6 @@
     <t>Prohibido reproducir sin  autorización</t>
   </si>
   <si>
-    <t>MÉTODO "A"</t>
-  </si>
-  <si>
-    <t>MÉTODO "B"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">g </t>
-  </si>
-  <si>
     <t>- La muestra de ensayo tiene una masa menor que la mínima requerida por la norma. (Si/No)</t>
   </si>
   <si>
@@ -163,9 +154,6 @@
     <t>Masa del recipiente</t>
   </si>
   <si>
-    <t>MÉTODO MARQUE "X"</t>
-  </si>
-  <si>
     <t>DESCRIPCIÓN</t>
   </si>
   <si>
@@ -178,9 +166,6 @@
     <t>Descripción de la muestra</t>
   </si>
   <si>
-    <t>Descripción material excluido: …....................................................................................................</t>
-  </si>
-  <si>
     <t>Método A</t>
   </si>
   <si>
@@ -269,6 +254,30 @@
   </si>
   <si>
     <t>REALIZADO</t>
+  </si>
+  <si>
+    <t>MUESTRA01</t>
+  </si>
+  <si>
+    <t>CONDICION01</t>
+  </si>
+  <si>
+    <t>1 1/2</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>MÉTODO PRUEBA</t>
+  </si>
+  <si>
+    <t>MÉTODO "A" o "B"</t>
+  </si>
+  <si>
+    <t>Forma de la partìcula:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descripción material excluido: </t>
   </si>
 </sst>
 </file>
@@ -676,7 +685,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -813,15 +822,6 @@
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
@@ -1003,17 +1003,51 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1103,17 +1137,26 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1131,10 +1174,10 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -1157,12 +1200,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1378,7 +1415,7 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>Revisado:</a:t>
+            <a:t>Revisado: angel</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1402,7 +1439,7 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>Fecha:</a:t>
+            <a:t>Fecha: 04/11/26</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1474,7 +1511,7 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>Aprobado:</a:t>
+            <a:t>Aprobado: JAZMIN</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1498,7 +1535,7 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>Fecha:</a:t>
+            <a:t>Fecha: 02/02/26</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1564,258 +1601,6 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>251460</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>526732</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>16193</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Rectángulo 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3450E0D-4F26-4E52-9FCC-E3A986384AD2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="3543300" y="1371600"/>
-          <a:ext cx="1258252" cy="221933"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="12700">
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr" upright="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="es-PE" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>144780</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>992777</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>16193</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="Rectángulo 10">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{443FDFFB-FF16-49CE-8274-3A3549CBB661}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="5069477" y="1380309"/>
-          <a:ext cx="847997" cy="225198"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="12700">
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr" upright="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="es-PE" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>622663</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>8709</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>721723</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>33610</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="Rectángulo 12">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{325CB4C3-5063-4F15-B269-4F3E096A533B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1432560" y="1397726"/>
-          <a:ext cx="847997" cy="225198"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="12700">
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr" upright="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="es-PE" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>971007</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>77289</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="Rectángulo 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5F863DF-5F5E-4CAF-97F2-E3D55EF4B1DB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="2529841" y="1389017"/>
-          <a:ext cx="847997" cy="230777"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="12700">
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr" upright="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="es-PE" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2251,8 +2036,8 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:W63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="175" zoomScaleNormal="100" zoomScaleSheetLayoutView="175" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:L8"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="Q49" sqref="Q49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.33203125" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2354,36 +2139,36 @@
       <c r="L6" s="26"/>
     </row>
     <row r="7" spans="1:13" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="123" t="s">
+      <c r="A7" s="130" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="123"/>
-      <c r="C7" s="123"/>
-      <c r="D7" s="123"/>
-      <c r="E7" s="123"/>
-      <c r="F7" s="123"/>
-      <c r="G7" s="123"/>
-      <c r="H7" s="123"/>
-      <c r="I7" s="123"/>
-      <c r="J7" s="123"/>
-      <c r="K7" s="123"/>
-      <c r="L7" s="123"/>
+      <c r="B7" s="130"/>
+      <c r="C7" s="130"/>
+      <c r="D7" s="130"/>
+      <c r="E7" s="130"/>
+      <c r="F7" s="130"/>
+      <c r="G7" s="130"/>
+      <c r="H7" s="130"/>
+      <c r="I7" s="130"/>
+      <c r="J7" s="130"/>
+      <c r="K7" s="130"/>
+      <c r="L7" s="130"/>
     </row>
     <row r="8" spans="1:13" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="124" t="s">
+      <c r="A8" s="131" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="124"/>
-      <c r="C8" s="124"/>
-      <c r="D8" s="124"/>
-      <c r="E8" s="124"/>
-      <c r="F8" s="124"/>
-      <c r="G8" s="124"/>
-      <c r="H8" s="124"/>
-      <c r="I8" s="124"/>
-      <c r="J8" s="124"/>
-      <c r="K8" s="124"/>
-      <c r="L8" s="124"/>
+      <c r="B8" s="131"/>
+      <c r="C8" s="131"/>
+      <c r="D8" s="131"/>
+      <c r="E8" s="131"/>
+      <c r="F8" s="131"/>
+      <c r="G8" s="131"/>
+      <c r="H8" s="131"/>
+      <c r="I8" s="131"/>
+      <c r="J8" s="131"/>
+      <c r="K8" s="131"/>
+      <c r="L8" s="131"/>
     </row>
     <row r="9" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27"/>
@@ -2402,19 +2187,19 @@
     <row r="10" spans="1:13" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="27"/>
       <c r="B10" s="27"/>
-      <c r="D10" s="147" t="s">
-        <v>74</v>
-      </c>
-      <c r="E10" s="146" t="s">
-        <v>75</v>
-      </c>
-      <c r="F10" s="27"/>
-      <c r="G10" s="146" t="s">
-        <v>76</v>
-      </c>
-      <c r="H10" s="27"/>
-      <c r="I10" s="146" t="s">
-        <v>77</v>
+      <c r="D10" s="110" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="110" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" s="111"/>
+      <c r="G10" s="112" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" s="113"/>
+      <c r="I10" s="110" t="s">
+        <v>72</v>
       </c>
       <c r="J10" s="27"/>
       <c r="K10" s="27"/>
@@ -2424,12 +2209,12 @@
       <c r="A11" s="27"/>
       <c r="B11" s="27"/>
       <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
+      <c r="D11" s="110"/>
+      <c r="E11" s="110"/>
+      <c r="F11" s="111"/>
+      <c r="G11" s="112"/>
+      <c r="H11" s="113"/>
+      <c r="I11" s="110"/>
       <c r="J11" s="27"/>
       <c r="K11" s="27"/>
       <c r="L11" s="27"/>
@@ -2438,12 +2223,8 @@
       <c r="A12" s="27"/>
       <c r="B12" s="27"/>
       <c r="C12" s="27"/>
-      <c r="D12"/>
-      <c r="E12"/>
       <c r="F12"/>
-      <c r="G12"/>
       <c r="H12"/>
-      <c r="I12"/>
       <c r="J12" s="27"/>
       <c r="K12" s="27"/>
       <c r="L12" s="27"/>
@@ -2464,37 +2245,37 @@
       <c r="M13" s="32"/>
     </row>
     <row r="14" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="125" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="126"/>
-      <c r="C14" s="126"/>
-      <c r="D14" s="126"/>
-      <c r="E14" s="126"/>
-      <c r="F14" s="126"/>
-      <c r="G14" s="126"/>
-      <c r="H14" s="126"/>
-      <c r="I14" s="126"/>
-      <c r="J14" s="126"/>
-      <c r="K14" s="126"/>
-      <c r="L14" s="127"/>
+      <c r="A14" s="132" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="133"/>
+      <c r="C14" s="133"/>
+      <c r="D14" s="133"/>
+      <c r="E14" s="133"/>
+      <c r="F14" s="133"/>
+      <c r="G14" s="133"/>
+      <c r="H14" s="133"/>
+      <c r="I14" s="133"/>
+      <c r="J14" s="133"/>
+      <c r="K14" s="133"/>
+      <c r="L14" s="134"/>
       <c r="M14" s="32"/>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="134" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="135"/>
-      <c r="C15" s="135"/>
-      <c r="D15" s="135"/>
-      <c r="E15" s="135"/>
-      <c r="F15" s="135"/>
-      <c r="G15" s="135"/>
-      <c r="H15" s="135"/>
-      <c r="I15" s="135"/>
-      <c r="J15" s="135"/>
-      <c r="K15" s="135"/>
-      <c r="L15" s="136"/>
+      <c r="A15" s="144" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="145"/>
+      <c r="C15" s="145"/>
+      <c r="D15" s="145"/>
+      <c r="E15" s="145"/>
+      <c r="F15" s="145"/>
+      <c r="G15" s="145"/>
+      <c r="H15" s="145"/>
+      <c r="I15" s="145"/>
+      <c r="J15" s="145"/>
+      <c r="K15" s="145"/>
+      <c r="L15" s="146"/>
       <c r="M15" s="32"/>
     </row>
     <row r="16" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2513,24 +2294,24 @@
       <c r="M16" s="32"/>
     </row>
     <row r="17" spans="1:19" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="128" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="129"/>
-      <c r="C17" s="129"/>
-      <c r="D17" s="129"/>
-      <c r="E17" s="129"/>
-      <c r="F17" s="129"/>
-      <c r="G17" s="129"/>
-      <c r="H17" s="129"/>
-      <c r="I17" s="129"/>
+      <c r="A17" s="135" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="136"/>
+      <c r="C17" s="136"/>
+      <c r="D17" s="136"/>
+      <c r="E17" s="136"/>
+      <c r="F17" s="136"/>
+      <c r="G17" s="136"/>
+      <c r="H17" s="136"/>
+      <c r="I17" s="136"/>
       <c r="J17" s="37"/>
       <c r="K17" s="37"/>
       <c r="L17" s="38"/>
     </row>
     <row r="18" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="39" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B18" s="40"/>
       <c r="C18" s="40"/>
@@ -2540,13 +2321,13 @@
       <c r="G18" s="40"/>
       <c r="H18" s="40"/>
       <c r="I18" s="40"/>
-      <c r="J18" s="102"/>
+      <c r="J18" s="99"/>
       <c r="K18" s="37"/>
       <c r="L18" s="38"/>
     </row>
     <row r="19" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="39" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B19" s="40"/>
       <c r="C19" s="40"/>
@@ -2556,13 +2337,13 @@
       <c r="G19" s="40"/>
       <c r="H19" s="40"/>
       <c r="I19" s="40"/>
-      <c r="J19" s="102"/>
+      <c r="J19" s="99"/>
       <c r="K19" s="37"/>
       <c r="L19" s="38"/>
     </row>
     <row r="20" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="39" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B20" s="40"/>
       <c r="C20" s="40"/>
@@ -2572,13 +2353,13 @@
       <c r="G20" s="40"/>
       <c r="H20" s="40"/>
       <c r="I20" s="40"/>
-      <c r="J20" s="102"/>
+      <c r="J20" s="99"/>
       <c r="K20" s="37"/>
       <c r="L20" s="38"/>
     </row>
     <row r="21" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="39" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B21" s="40"/>
       <c r="C21" s="40"/>
@@ -2588,13 +2369,13 @@
       <c r="G21" s="40"/>
       <c r="H21" s="40"/>
       <c r="I21" s="40"/>
-      <c r="J21" s="102"/>
+      <c r="J21" s="99"/>
       <c r="K21" s="37"/>
       <c r="L21" s="38"/>
     </row>
     <row r="22" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="41" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="B22" s="40"/>
       <c r="C22" s="40"/>
@@ -2623,704 +2404,716 @@
       <c r="L23" s="38"/>
     </row>
     <row r="24" spans="1:19" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="128" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="129"/>
-      <c r="C24" s="129"/>
-      <c r="D24" s="129"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="43"/>
-      <c r="I24" s="43"/>
-      <c r="J24" s="37"/>
+      <c r="A24" s="137" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="138"/>
+      <c r="C24" s="138"/>
+      <c r="D24" s="138"/>
+      <c r="E24" s="102"/>
+      <c r="F24" s="102"/>
+      <c r="G24" s="102"/>
+      <c r="H24" s="102"/>
+      <c r="I24" s="102"/>
+      <c r="J24" s="103"/>
       <c r="K24" s="37"/>
       <c r="L24" s="38"/>
     </row>
     <row r="25" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="138" t="s">
-        <v>37</v>
-      </c>
-      <c r="B25" s="138"/>
-      <c r="C25" s="138"/>
-      <c r="D25" s="138"/>
-      <c r="E25" s="139"/>
-      <c r="F25" s="139"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="131" t="s">
-        <v>42</v>
-      </c>
-      <c r="I25" s="132"/>
-      <c r="J25" s="133"/>
+      <c r="A25" s="148" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="148"/>
+      <c r="C25" s="148"/>
+      <c r="D25" s="148"/>
+      <c r="E25" s="149" t="s">
+        <v>73</v>
+      </c>
+      <c r="F25" s="149"/>
+      <c r="G25" s="104"/>
+      <c r="H25" s="140" t="s">
+        <v>77</v>
+      </c>
+      <c r="I25" s="141"/>
+      <c r="J25" s="142"/>
       <c r="K25" s="45"/>
       <c r="L25" s="38"/>
     </row>
     <row r="26" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="138" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="138"/>
-      <c r="C26" s="138"/>
-      <c r="D26" s="138"/>
-      <c r="E26" s="139"/>
-      <c r="F26" s="139"/>
-      <c r="G26" s="44"/>
-      <c r="H26" s="131" t="s">
-        <v>31</v>
-      </c>
-      <c r="I26" s="133"/>
-      <c r="J26" s="103"/>
+      <c r="A26" s="148" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="148"/>
+      <c r="C26" s="148"/>
+      <c r="D26" s="148"/>
+      <c r="E26" s="149" t="s">
+        <v>74</v>
+      </c>
+      <c r="F26" s="149"/>
+      <c r="G26" s="104"/>
+      <c r="H26" s="143" t="s">
+        <v>78</v>
+      </c>
+      <c r="I26" s="143"/>
+      <c r="J26" s="105"/>
       <c r="K26" s="46"/>
       <c r="L26" s="38"/>
     </row>
     <row r="27" spans="1:19" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="138" t="s">
-        <v>67</v>
-      </c>
-      <c r="B27" s="138"/>
-      <c r="C27" s="138"/>
-      <c r="D27" s="138"/>
-      <c r="E27" s="139"/>
-      <c r="F27" s="139"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="131" t="s">
-        <v>32</v>
-      </c>
-      <c r="I27" s="133"/>
-      <c r="J27" s="103"/>
-      <c r="K27" s="46"/>
+      <c r="A27" s="148" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="148"/>
+      <c r="C27" s="148"/>
+      <c r="D27" s="148"/>
+      <c r="E27" s="149" t="s">
+        <v>75</v>
+      </c>
+      <c r="F27" s="149"/>
+      <c r="G27" s="104"/>
+      <c r="H27" s="106"/>
+      <c r="I27" s="107"/>
+      <c r="J27" s="108"/>
+      <c r="K27" s="108"/>
       <c r="L27" s="38"/>
       <c r="M27" s="32"/>
     </row>
     <row r="28" spans="1:19" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="47"/>
-      <c r="B28" s="48"/>
-      <c r="C28" s="48"/>
-      <c r="D28" s="49"/>
-      <c r="L28" s="50"/>
+      <c r="A28" s="148" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" s="148"/>
+      <c r="C28" s="148"/>
+      <c r="D28" s="148"/>
+      <c r="E28" s="149"/>
+      <c r="F28" s="149"/>
+      <c r="G28" s="109"/>
+      <c r="H28" s="109"/>
+      <c r="I28" s="109"/>
+      <c r="J28" s="109"/>
+      <c r="L28" s="47"/>
       <c r="M28" s="32"/>
     </row>
     <row r="29" spans="1:19" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="51"/>
-      <c r="B29" s="52"/>
-      <c r="C29" s="52"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="52"/>
-      <c r="F29" s="52"/>
-      <c r="G29" s="53"/>
-      <c r="H29" s="53"/>
-      <c r="I29" s="53"/>
-      <c r="J29" s="54"/>
-      <c r="K29" s="54"/>
-      <c r="L29" s="55"/>
+      <c r="A29" s="48"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="51"/>
+      <c r="K29" s="51"/>
+      <c r="L29" s="52"/>
       <c r="M29" s="32"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="56"/>
-      <c r="B30" s="130" t="s">
+      <c r="A30" s="53"/>
+      <c r="B30" s="139" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="139"/>
+      <c r="D30" s="139"/>
+      <c r="E30" s="139"/>
+      <c r="F30" s="139"/>
+      <c r="G30" s="139"/>
+      <c r="H30" s="54" t="s">
+        <v>40</v>
+      </c>
+      <c r="I30" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="J30" s="147"/>
+      <c r="K30" s="147"/>
+      <c r="L30" s="55"/>
+      <c r="M30" s="32"/>
+    </row>
+    <row r="31" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="56"/>
+      <c r="B31" s="57">
+        <v>1</v>
+      </c>
+      <c r="C31" s="151" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="152"/>
+      <c r="E31" s="152"/>
+      <c r="F31" s="152"/>
+      <c r="G31" s="153"/>
+      <c r="H31" s="58" t="s">
+        <v>18</v>
+      </c>
+      <c r="I31" s="101"/>
+      <c r="J31" s="59"/>
+      <c r="K31" s="59"/>
+      <c r="L31" s="60"/>
+      <c r="M31" s="32"/>
+    </row>
+    <row r="32" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="56"/>
+      <c r="B32" s="61">
+        <v>2</v>
+      </c>
+      <c r="C32" s="151" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="152"/>
+      <c r="E32" s="152"/>
+      <c r="F32" s="152"/>
+      <c r="G32" s="153"/>
+      <c r="H32" s="58" t="s">
+        <v>18</v>
+      </c>
+      <c r="I32" s="100"/>
+      <c r="J32" s="59"/>
+      <c r="K32" s="59"/>
+      <c r="L32" s="60"/>
+      <c r="M32" s="32"/>
+      <c r="S32" s="63"/>
+    </row>
+    <row r="33" spans="1:23" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="56"/>
+      <c r="B33" s="61">
+        <v>3</v>
+      </c>
+      <c r="C33" s="151" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="152"/>
+      <c r="E33" s="152"/>
+      <c r="F33" s="152"/>
+      <c r="G33" s="153"/>
+      <c r="H33" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="I33" s="100"/>
+      <c r="J33" s="59"/>
+      <c r="K33" s="59"/>
+      <c r="L33" s="64"/>
+      <c r="M33" s="65"/>
+      <c r="W33" s="63"/>
+    </row>
+    <row r="34" spans="1:23" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="56"/>
+      <c r="B34" s="57">
+        <v>4</v>
+      </c>
+      <c r="C34" s="151" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" s="152"/>
+      <c r="E34" s="152"/>
+      <c r="F34" s="152"/>
+      <c r="G34" s="153"/>
+      <c r="H34" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="I34" s="100"/>
+      <c r="J34" s="59"/>
+      <c r="K34" s="59"/>
+      <c r="L34" s="64"/>
+      <c r="M34" s="65"/>
+      <c r="O34" s="62"/>
+      <c r="P34" s="62"/>
+      <c r="W34" s="63"/>
+    </row>
+    <row r="35" spans="1:23" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="56"/>
+      <c r="B35" s="61">
+        <v>5</v>
+      </c>
+      <c r="C35" s="151" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="152"/>
+      <c r="E35" s="152"/>
+      <c r="F35" s="152"/>
+      <c r="G35" s="153"/>
+      <c r="H35" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="I35" s="100"/>
+      <c r="J35" s="59"/>
+      <c r="K35" s="59"/>
+      <c r="L35" s="66"/>
+      <c r="M35" s="65"/>
+      <c r="O35" s="62"/>
+      <c r="P35" s="62"/>
+      <c r="W35" s="63"/>
+    </row>
+    <row r="36" spans="1:23" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="56"/>
+      <c r="B36" s="57">
+        <v>6</v>
+      </c>
+      <c r="C36" s="151" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="152"/>
+      <c r="E36" s="152"/>
+      <c r="F36" s="152"/>
+      <c r="G36" s="153"/>
+      <c r="H36" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="I36" s="100"/>
+      <c r="J36" s="59"/>
+      <c r="K36" s="59"/>
+      <c r="L36" s="66"/>
+      <c r="M36" s="65"/>
+      <c r="O36" s="62"/>
+      <c r="P36" s="62"/>
+      <c r="W36" s="63"/>
+    </row>
+    <row r="37" spans="1:23" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="56"/>
+      <c r="B37" s="61">
+        <v>7</v>
+      </c>
+      <c r="C37" s="151" t="s">
+        <v>58</v>
+      </c>
+      <c r="D37" s="152"/>
+      <c r="E37" s="152"/>
+      <c r="F37" s="152"/>
+      <c r="G37" s="153"/>
+      <c r="H37" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="I37" s="100"/>
+      <c r="J37" s="59"/>
+      <c r="K37" s="59"/>
+      <c r="L37" s="66"/>
+      <c r="M37" s="65"/>
+      <c r="N37" s="67"/>
+      <c r="O37" s="62"/>
+      <c r="P37" s="62"/>
+    </row>
+    <row r="38" spans="1:23" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="56"/>
+      <c r="B38" s="61">
+        <v>8</v>
+      </c>
+      <c r="C38" s="151" t="s">
+        <v>59</v>
+      </c>
+      <c r="D38" s="152"/>
+      <c r="E38" s="152"/>
+      <c r="F38" s="152"/>
+      <c r="G38" s="153"/>
+      <c r="H38" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="I38" s="100"/>
+      <c r="J38" s="59"/>
+      <c r="K38" s="59"/>
+      <c r="L38" s="66"/>
+      <c r="M38" s="65"/>
+      <c r="N38" s="68"/>
+      <c r="O38" s="69"/>
+      <c r="P38" s="69"/>
+    </row>
+    <row r="39" spans="1:23" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="56"/>
+      <c r="B39" s="57">
+        <v>9</v>
+      </c>
+      <c r="C39" s="151" t="s">
+        <v>60</v>
+      </c>
+      <c r="D39" s="152"/>
+      <c r="E39" s="152"/>
+      <c r="F39" s="152"/>
+      <c r="G39" s="153"/>
+      <c r="H39" s="58" t="s">
+        <v>19</v>
+      </c>
+      <c r="I39" s="100"/>
+      <c r="J39" s="59"/>
+      <c r="K39" s="59"/>
+      <c r="L39" s="66"/>
+      <c r="M39" s="65"/>
+      <c r="N39" s="70"/>
+      <c r="O39" s="71"/>
+    </row>
+    <row r="40" spans="1:23" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="56"/>
+      <c r="B40" s="50"/>
+      <c r="C40" s="50"/>
+      <c r="D40" s="50"/>
+      <c r="E40" s="50"/>
+      <c r="F40" s="50"/>
+      <c r="I40" s="72"/>
+      <c r="J40" s="73"/>
+      <c r="K40" s="73"/>
+      <c r="L40" s="66"/>
+      <c r="M40" s="32"/>
+      <c r="N40" s="70"/>
+      <c r="O40" s="71"/>
+      <c r="W40" s="63"/>
+    </row>
+    <row r="41" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="56"/>
+      <c r="B41" s="127" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="130"/>
-      <c r="D30" s="130"/>
-      <c r="E30" s="130"/>
-      <c r="F30" s="130"/>
-      <c r="G30" s="130"/>
-      <c r="H30" s="57" t="s">
+      <c r="C41" s="127"/>
+      <c r="D41" s="127"/>
+      <c r="E41" s="127"/>
+      <c r="F41" s="127"/>
+      <c r="G41" s="74"/>
+      <c r="H41" s="116" t="s">
+        <v>26</v>
+      </c>
+      <c r="I41" s="117"/>
+      <c r="J41" s="150"/>
+      <c r="K41" s="150"/>
+      <c r="L41" s="117"/>
+      <c r="M41" s="32"/>
+      <c r="W41" s="63"/>
+    </row>
+    <row r="42" spans="1:23" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="56"/>
+      <c r="B42" s="128" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" s="128"/>
+      <c r="D42" s="128"/>
+      <c r="E42" s="75" t="s">
+        <v>48</v>
+      </c>
+      <c r="F42" s="75" t="s">
+        <v>63</v>
+      </c>
+      <c r="G42" s="74"/>
+      <c r="H42" s="126" t="s">
+        <v>27</v>
+      </c>
+      <c r="I42" s="126"/>
+      <c r="J42" s="125"/>
+      <c r="K42" s="125"/>
+      <c r="L42" s="125"/>
+      <c r="M42" s="32"/>
+      <c r="W42" s="63"/>
+    </row>
+    <row r="43" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="56"/>
+      <c r="B43" s="129" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" s="129"/>
+      <c r="D43" s="129"/>
+      <c r="E43" s="76" t="s">
+        <v>23</v>
+      </c>
+      <c r="F43" s="76" t="s">
+        <v>64</v>
+      </c>
+      <c r="G43" s="74"/>
+      <c r="H43" s="126" t="s">
+        <v>28</v>
+      </c>
+      <c r="I43" s="126"/>
+      <c r="J43" s="118"/>
+      <c r="K43" s="118"/>
+      <c r="L43" s="119"/>
+      <c r="M43" s="32"/>
+      <c r="W43" s="63"/>
+    </row>
+    <row r="44" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="56"/>
+      <c r="B44" s="129" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" s="129"/>
+      <c r="D44" s="129"/>
+      <c r="E44" s="76" t="s">
+        <v>22</v>
+      </c>
+      <c r="F44" s="76" t="s">
+        <v>64</v>
+      </c>
+      <c r="G44" s="74"/>
+      <c r="H44" s="126"/>
+      <c r="I44" s="126"/>
+      <c r="J44" s="120"/>
+      <c r="K44" s="120"/>
+      <c r="L44" s="121"/>
+      <c r="M44" s="32"/>
+    </row>
+    <row r="45" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="56"/>
+      <c r="B45" s="154" t="s">
+        <v>54</v>
+      </c>
+      <c r="C45" s="154"/>
+      <c r="D45" s="154"/>
+      <c r="E45" s="76" t="s">
+        <v>21</v>
+      </c>
+      <c r="F45" s="76" t="s">
+        <v>64</v>
+      </c>
+      <c r="G45" s="74"/>
+      <c r="H45" s="126" t="s">
+        <v>29</v>
+      </c>
+      <c r="I45" s="126"/>
+      <c r="J45" s="118"/>
+      <c r="K45" s="118"/>
+      <c r="L45" s="119"/>
+      <c r="M45" s="32"/>
+    </row>
+    <row r="46" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="56"/>
+      <c r="B46" s="127" t="s">
         <v>44</v>
       </c>
-      <c r="I30" s="57" t="s">
+      <c r="C46" s="127"/>
+      <c r="D46" s="127"/>
+      <c r="E46" s="127"/>
+      <c r="F46" s="127"/>
+      <c r="G46" s="74"/>
+      <c r="H46" s="126"/>
+      <c r="I46" s="126"/>
+      <c r="J46" s="120"/>
+      <c r="K46" s="120"/>
+      <c r="L46" s="121"/>
+      <c r="M46" s="32"/>
+    </row>
+    <row r="47" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="56"/>
+      <c r="B47" s="154" t="s">
+        <v>55</v>
+      </c>
+      <c r="C47" s="154"/>
+      <c r="D47" s="154"/>
+      <c r="E47" s="76" t="s">
+        <v>20</v>
+      </c>
+      <c r="F47" s="76" t="s">
+        <v>65</v>
+      </c>
+      <c r="G47" s="74"/>
+      <c r="H47" s="122"/>
+      <c r="I47" s="122"/>
+      <c r="J47" s="123"/>
+      <c r="K47" s="123"/>
+      <c r="L47" s="124"/>
+      <c r="M47" s="32"/>
+    </row>
+    <row r="48" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="56"/>
+      <c r="B48" s="129" t="s">
+        <v>50</v>
+      </c>
+      <c r="C48" s="129"/>
+      <c r="D48" s="129"/>
+      <c r="E48" s="76" t="s">
+        <v>21</v>
+      </c>
+      <c r="F48" s="76" t="s">
+        <v>65</v>
+      </c>
+      <c r="G48" s="74"/>
+      <c r="H48" s="122"/>
+      <c r="I48" s="122"/>
+      <c r="J48" s="123"/>
+      <c r="K48" s="123"/>
+      <c r="L48" s="124"/>
+      <c r="M48" s="32"/>
+    </row>
+    <row r="49" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="56"/>
+      <c r="B49" s="129" t="s">
+        <v>51</v>
+      </c>
+      <c r="C49" s="129"/>
+      <c r="D49" s="129"/>
+      <c r="E49" s="76" t="s">
+        <v>21</v>
+      </c>
+      <c r="F49" s="76" t="s">
+        <v>65</v>
+      </c>
+      <c r="G49" s="74"/>
+      <c r="H49" s="77"/>
+      <c r="I49" s="77"/>
+      <c r="J49" s="78"/>
+      <c r="K49" s="78"/>
+      <c r="L49" s="79"/>
+      <c r="M49" s="32"/>
+    </row>
+    <row r="50" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="80"/>
+      <c r="B50" s="81" t="s">
         <v>66</v>
       </c>
-      <c r="J30" s="137"/>
-      <c r="K30" s="137"/>
-      <c r="L30" s="58"/>
-      <c r="M30" s="32"/>
-    </row>
-    <row r="31" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="59"/>
-      <c r="B31" s="60">
-        <v>1</v>
-      </c>
-      <c r="C31" s="141" t="s">
-        <v>17</v>
-      </c>
-      <c r="D31" s="142"/>
-      <c r="E31" s="142"/>
-      <c r="F31" s="142"/>
-      <c r="G31" s="143"/>
-      <c r="H31" s="61" t="s">
-        <v>18</v>
-      </c>
-      <c r="I31" s="106"/>
-      <c r="J31" s="62"/>
-      <c r="K31" s="62"/>
-      <c r="L31" s="63"/>
-      <c r="M31" s="32"/>
-    </row>
-    <row r="32" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="59"/>
-      <c r="B32" s="64">
-        <v>2</v>
-      </c>
-      <c r="C32" s="141" t="s">
-        <v>39</v>
-      </c>
-      <c r="D32" s="142"/>
-      <c r="E32" s="142"/>
-      <c r="F32" s="142"/>
-      <c r="G32" s="143"/>
-      <c r="H32" s="61" t="s">
-        <v>18</v>
-      </c>
-      <c r="I32" s="104"/>
-      <c r="J32" s="62"/>
-      <c r="K32" s="62"/>
-      <c r="L32" s="63"/>
-      <c r="M32" s="32"/>
-      <c r="S32" s="66"/>
-    </row>
-    <row r="33" spans="1:23" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="59"/>
-      <c r="B33" s="64">
-        <v>3</v>
-      </c>
-      <c r="C33" s="141" t="s">
-        <v>40</v>
-      </c>
-      <c r="D33" s="142"/>
-      <c r="E33" s="142"/>
-      <c r="F33" s="142"/>
-      <c r="G33" s="143"/>
-      <c r="H33" s="61" t="s">
-        <v>33</v>
-      </c>
-      <c r="I33" s="104"/>
-      <c r="J33" s="62"/>
-      <c r="K33" s="62"/>
-      <c r="L33" s="67"/>
-      <c r="M33" s="68"/>
-      <c r="W33" s="66"/>
-    </row>
-    <row r="34" spans="1:23" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="59"/>
-      <c r="B34" s="60">
-        <v>4</v>
-      </c>
-      <c r="C34" s="141" t="s">
-        <v>61</v>
-      </c>
-      <c r="D34" s="142"/>
-      <c r="E34" s="142"/>
-      <c r="F34" s="142"/>
-      <c r="G34" s="143"/>
-      <c r="H34" s="61" t="s">
-        <v>33</v>
-      </c>
-      <c r="I34" s="104"/>
-      <c r="J34" s="62"/>
-      <c r="K34" s="62"/>
-      <c r="L34" s="67"/>
-      <c r="M34" s="68"/>
-      <c r="O34" s="65"/>
-      <c r="P34" s="65"/>
-      <c r="W34" s="66"/>
-    </row>
-    <row r="35" spans="1:23" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="59"/>
-      <c r="B35" s="64">
-        <v>5</v>
-      </c>
-      <c r="C35" s="141" t="s">
-        <v>62</v>
-      </c>
-      <c r="D35" s="142"/>
-      <c r="E35" s="142"/>
-      <c r="F35" s="142"/>
-      <c r="G35" s="143"/>
-      <c r="H35" s="61" t="s">
-        <v>33</v>
-      </c>
-      <c r="I35" s="104"/>
-      <c r="J35" s="62"/>
-      <c r="K35" s="62"/>
-      <c r="L35" s="69"/>
-      <c r="M35" s="68"/>
-      <c r="O35" s="65"/>
-      <c r="P35" s="65"/>
-      <c r="W35" s="66"/>
-    </row>
-    <row r="36" spans="1:23" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="59"/>
-      <c r="B36" s="60">
-        <v>6</v>
-      </c>
-      <c r="C36" s="141" t="s">
-        <v>41</v>
-      </c>
-      <c r="D36" s="142"/>
-      <c r="E36" s="142"/>
-      <c r="F36" s="142"/>
-      <c r="G36" s="143"/>
-      <c r="H36" s="61" t="s">
-        <v>33</v>
-      </c>
-      <c r="I36" s="104"/>
-      <c r="J36" s="62"/>
-      <c r="K36" s="62"/>
-      <c r="L36" s="69"/>
-      <c r="M36" s="68"/>
-      <c r="O36" s="65"/>
-      <c r="P36" s="65"/>
-      <c r="W36" s="66"/>
-    </row>
-    <row r="37" spans="1:23" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="59"/>
-      <c r="B37" s="64">
-        <v>7</v>
-      </c>
-      <c r="C37" s="141" t="s">
-        <v>63</v>
-      </c>
-      <c r="D37" s="142"/>
-      <c r="E37" s="142"/>
-      <c r="F37" s="142"/>
-      <c r="G37" s="143"/>
-      <c r="H37" s="61" t="s">
-        <v>33</v>
-      </c>
-      <c r="I37" s="105"/>
-      <c r="J37" s="62"/>
-      <c r="K37" s="62"/>
-      <c r="L37" s="69"/>
-      <c r="M37" s="68"/>
-      <c r="N37" s="70"/>
-      <c r="O37" s="65"/>
-      <c r="P37" s="65"/>
-    </row>
-    <row r="38" spans="1:23" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="59"/>
-      <c r="B38" s="64">
-        <v>8</v>
-      </c>
-      <c r="C38" s="141" t="s">
-        <v>64</v>
-      </c>
-      <c r="D38" s="142"/>
-      <c r="E38" s="142"/>
-      <c r="F38" s="142"/>
-      <c r="G38" s="143"/>
-      <c r="H38" s="61" t="s">
-        <v>33</v>
-      </c>
-      <c r="I38" s="105"/>
-      <c r="J38" s="62"/>
-      <c r="K38" s="62"/>
-      <c r="L38" s="69"/>
-      <c r="M38" s="68"/>
-      <c r="N38" s="71"/>
-      <c r="O38" s="72"/>
-      <c r="P38" s="72"/>
-    </row>
-    <row r="39" spans="1:23" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="59"/>
-      <c r="B39" s="60">
-        <v>9</v>
-      </c>
-      <c r="C39" s="141" t="s">
-        <v>65</v>
-      </c>
-      <c r="D39" s="142"/>
-      <c r="E39" s="142"/>
-      <c r="F39" s="142"/>
-      <c r="G39" s="143"/>
-      <c r="H39" s="61" t="s">
-        <v>19</v>
-      </c>
-      <c r="I39" s="105"/>
-      <c r="J39" s="62"/>
-      <c r="K39" s="62"/>
-      <c r="L39" s="69"/>
-      <c r="M39" s="68"/>
-      <c r="N39" s="73"/>
-      <c r="O39" s="74"/>
-    </row>
-    <row r="40" spans="1:23" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="59"/>
-      <c r="B40" s="53"/>
-      <c r="C40" s="53"/>
-      <c r="D40" s="53"/>
-      <c r="E40" s="53"/>
-      <c r="F40" s="53"/>
-      <c r="I40" s="75"/>
-      <c r="J40" s="76"/>
-      <c r="K40" s="76"/>
-      <c r="L40" s="69"/>
-      <c r="M40" s="32"/>
-      <c r="N40" s="73"/>
-      <c r="O40" s="74"/>
-      <c r="W40" s="66"/>
-    </row>
-    <row r="41" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="59"/>
-      <c r="B41" s="120" t="s">
-        <v>48</v>
-      </c>
-      <c r="C41" s="120"/>
-      <c r="D41" s="120"/>
-      <c r="E41" s="120"/>
-      <c r="F41" s="120"/>
-      <c r="G41" s="77"/>
-      <c r="H41" s="109" t="s">
-        <v>26</v>
-      </c>
-      <c r="I41" s="110"/>
-      <c r="J41" s="140"/>
-      <c r="K41" s="140"/>
-      <c r="L41" s="110"/>
-      <c r="M41" s="32"/>
-      <c r="W41" s="66"/>
-    </row>
-    <row r="42" spans="1:23" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="59"/>
-      <c r="B42" s="121" t="s">
-        <v>54</v>
-      </c>
-      <c r="C42" s="121"/>
-      <c r="D42" s="121"/>
-      <c r="E42" s="78" t="s">
-        <v>53</v>
-      </c>
-      <c r="F42" s="78" t="s">
-        <v>68</v>
-      </c>
-      <c r="G42" s="77"/>
-      <c r="H42" s="119" t="s">
-        <v>27</v>
-      </c>
-      <c r="I42" s="119"/>
-      <c r="J42" s="118"/>
-      <c r="K42" s="118"/>
-      <c r="L42" s="118"/>
-      <c r="M42" s="32"/>
-      <c r="W42" s="66"/>
-    </row>
-    <row r="43" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="59"/>
-      <c r="B43" s="122" t="s">
-        <v>57</v>
-      </c>
-      <c r="C43" s="122"/>
-      <c r="D43" s="122"/>
-      <c r="E43" s="79" t="s">
-        <v>23</v>
-      </c>
-      <c r="F43" s="79" t="s">
-        <v>69</v>
-      </c>
-      <c r="G43" s="77"/>
-      <c r="H43" s="119" t="s">
-        <v>28</v>
-      </c>
-      <c r="I43" s="119"/>
-      <c r="J43" s="111"/>
-      <c r="K43" s="111"/>
-      <c r="L43" s="112"/>
-      <c r="M43" s="32"/>
-      <c r="W43" s="66"/>
-    </row>
-    <row r="44" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="59"/>
-      <c r="B44" s="122" t="s">
-        <v>58</v>
-      </c>
-      <c r="C44" s="122"/>
-      <c r="D44" s="122"/>
-      <c r="E44" s="79" t="s">
-        <v>22</v>
-      </c>
-      <c r="F44" s="79" t="s">
-        <v>69</v>
-      </c>
-      <c r="G44" s="77"/>
-      <c r="H44" s="119"/>
-      <c r="I44" s="119"/>
-      <c r="J44" s="113"/>
-      <c r="K44" s="113"/>
-      <c r="L44" s="114"/>
-      <c r="M44" s="32"/>
-    </row>
-    <row r="45" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="59"/>
-      <c r="B45" s="144" t="s">
-        <v>59</v>
-      </c>
-      <c r="C45" s="144"/>
-      <c r="D45" s="144"/>
-      <c r="E45" s="79" t="s">
-        <v>21</v>
-      </c>
-      <c r="F45" s="79" t="s">
-        <v>69</v>
-      </c>
-      <c r="G45" s="77"/>
-      <c r="H45" s="119" t="s">
-        <v>29</v>
-      </c>
-      <c r="I45" s="119"/>
-      <c r="J45" s="111"/>
-      <c r="K45" s="111"/>
-      <c r="L45" s="112"/>
-      <c r="M45" s="32"/>
-    </row>
-    <row r="46" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="59"/>
-      <c r="B46" s="120" t="s">
-        <v>49</v>
-      </c>
-      <c r="C46" s="120"/>
-      <c r="D46" s="120"/>
-      <c r="E46" s="120"/>
-      <c r="F46" s="120"/>
-      <c r="G46" s="77"/>
-      <c r="H46" s="119"/>
-      <c r="I46" s="119"/>
-      <c r="J46" s="113"/>
-      <c r="K46" s="113"/>
-      <c r="L46" s="114"/>
-      <c r="M46" s="32"/>
-    </row>
-    <row r="47" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="59"/>
-      <c r="B47" s="144" t="s">
-        <v>60</v>
-      </c>
-      <c r="C47" s="144"/>
-      <c r="D47" s="144"/>
-      <c r="E47" s="79" t="s">
-        <v>20</v>
-      </c>
-      <c r="F47" s="79" t="s">
-        <v>70</v>
-      </c>
-      <c r="G47" s="77"/>
-      <c r="H47" s="115"/>
-      <c r="I47" s="115"/>
-      <c r="J47" s="116"/>
-      <c r="K47" s="116"/>
-      <c r="L47" s="117"/>
-      <c r="M47" s="32"/>
-    </row>
-    <row r="48" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="59"/>
-      <c r="B48" s="122" t="s">
-        <v>55</v>
-      </c>
-      <c r="C48" s="122"/>
-      <c r="D48" s="122"/>
-      <c r="E48" s="79" t="s">
-        <v>21</v>
-      </c>
-      <c r="F48" s="79" t="s">
-        <v>70</v>
-      </c>
-      <c r="G48" s="77"/>
-      <c r="H48" s="115"/>
-      <c r="I48" s="115"/>
-      <c r="J48" s="116"/>
-      <c r="K48" s="116"/>
-      <c r="L48" s="117"/>
-      <c r="M48" s="32"/>
-    </row>
-    <row r="49" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="59"/>
-      <c r="B49" s="122" t="s">
-        <v>56</v>
-      </c>
-      <c r="C49" s="122"/>
-      <c r="D49" s="122"/>
-      <c r="E49" s="79" t="s">
-        <v>21</v>
-      </c>
-      <c r="F49" s="79" t="s">
-        <v>70</v>
-      </c>
-      <c r="G49" s="77"/>
-      <c r="H49" s="80"/>
-      <c r="I49" s="80"/>
-      <c r="J49" s="81"/>
-      <c r="K49" s="81"/>
-      <c r="L49" s="82"/>
-      <c r="M49" s="32"/>
-    </row>
-    <row r="50" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="83"/>
-      <c r="B50" s="84" t="s">
-        <v>71</v>
-      </c>
-      <c r="C50" s="85"/>
-      <c r="D50" s="85"/>
-      <c r="E50" s="86"/>
-      <c r="F50" s="86"/>
-      <c r="G50" s="87"/>
-      <c r="H50" s="88"/>
-      <c r="I50" s="88"/>
-      <c r="J50" s="89"/>
-      <c r="K50" s="89"/>
-      <c r="L50" s="90"/>
+      <c r="C50" s="82"/>
+      <c r="D50" s="82"/>
+      <c r="E50" s="83"/>
+      <c r="F50" s="83"/>
+      <c r="G50" s="84"/>
+      <c r="H50" s="85"/>
+      <c r="I50" s="85"/>
+      <c r="J50" s="86"/>
+      <c r="K50" s="86"/>
+      <c r="L50" s="87"/>
       <c r="M50" s="32"/>
     </row>
     <row r="51" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="91"/>
-      <c r="B51" s="66"/>
-      <c r="C51" s="66"/>
-      <c r="D51" s="66"/>
-      <c r="E51" s="66"/>
-      <c r="F51" s="66"/>
-      <c r="G51" s="66"/>
-      <c r="H51" s="92"/>
-      <c r="I51" s="93"/>
-      <c r="J51" s="66"/>
-      <c r="K51" s="66"/>
-      <c r="L51" s="66"/>
+      <c r="A51" s="88"/>
+      <c r="B51" s="63"/>
+      <c r="C51" s="63"/>
+      <c r="D51" s="63"/>
+      <c r="E51" s="63"/>
+      <c r="F51" s="63"/>
+      <c r="G51" s="63"/>
+      <c r="H51" s="89"/>
+      <c r="I51" s="90"/>
+      <c r="J51" s="63"/>
+      <c r="K51" s="63"/>
+      <c r="L51" s="63"/>
       <c r="M51" s="32"/>
     </row>
     <row r="52" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="94" t="s">
+      <c r="A52" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="B52" s="89"/>
-      <c r="C52" s="89"/>
-      <c r="D52" s="89"/>
-      <c r="E52" s="89"/>
-      <c r="F52" s="89"/>
-      <c r="G52" s="89"/>
-      <c r="H52" s="88"/>
-      <c r="I52" s="88"/>
-      <c r="J52" s="88"/>
-      <c r="K52" s="88"/>
-      <c r="L52" s="88"/>
+      <c r="B52" s="86"/>
+      <c r="C52" s="86"/>
+      <c r="D52" s="86"/>
+      <c r="E52" s="86"/>
+      <c r="F52" s="86"/>
+      <c r="G52" s="86"/>
+      <c r="H52" s="85"/>
+      <c r="I52" s="85"/>
+      <c r="J52" s="85"/>
+      <c r="K52" s="85"/>
+      <c r="L52" s="85"/>
       <c r="M52" s="32"/>
     </row>
     <row r="53" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="95"/>
-      <c r="B53" s="89"/>
-      <c r="C53" s="89"/>
-      <c r="D53" s="89"/>
-      <c r="E53" s="89"/>
-      <c r="F53" s="89"/>
-      <c r="G53" s="89"/>
-      <c r="H53" s="88"/>
-      <c r="I53" s="88"/>
-      <c r="J53" s="88"/>
-      <c r="K53" s="88"/>
-      <c r="L53" s="88"/>
+      <c r="A53" s="92"/>
+      <c r="B53" s="86"/>
+      <c r="C53" s="86"/>
+      <c r="D53" s="86"/>
+      <c r="E53" s="86"/>
+      <c r="F53" s="86"/>
+      <c r="G53" s="86"/>
+      <c r="H53" s="85"/>
+      <c r="I53" s="85"/>
+      <c r="J53" s="85"/>
+      <c r="K53" s="85"/>
+      <c r="L53" s="85"/>
       <c r="M53" s="32"/>
     </row>
     <row r="54" spans="1:13" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="96"/>
-      <c r="B54" s="66"/>
-      <c r="C54" s="66"/>
-      <c r="D54" s="66"/>
-      <c r="E54" s="66"/>
-      <c r="F54" s="66"/>
-      <c r="G54" s="66"/>
-      <c r="H54" s="97"/>
+      <c r="A54" s="93"/>
+      <c r="B54" s="63"/>
+      <c r="C54" s="63"/>
+      <c r="D54" s="63"/>
+      <c r="E54" s="63"/>
+      <c r="F54" s="63"/>
+      <c r="G54" s="63"/>
+      <c r="H54" s="94"/>
       <c r="I54" s="44"/>
-      <c r="J54" s="98"/>
-      <c r="K54" s="98"/>
-      <c r="L54" s="98"/>
+      <c r="J54" s="95"/>
+      <c r="K54" s="95"/>
+      <c r="L54" s="95"/>
       <c r="M54" s="32"/>
     </row>
     <row r="55" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="96"/>
-      <c r="B55" s="66"/>
-      <c r="C55" s="66"/>
-      <c r="D55" s="66"/>
-      <c r="E55" s="66"/>
-      <c r="F55" s="66"/>
-      <c r="G55" s="66"/>
-      <c r="H55" s="66"/>
-      <c r="I55" s="66"/>
-      <c r="J55" s="66"/>
-      <c r="K55" s="66"/>
-      <c r="L55" s="66"/>
+      <c r="A55" s="93"/>
+      <c r="B55" s="63"/>
+      <c r="C55" s="63"/>
+      <c r="D55" s="63"/>
+      <c r="E55" s="63"/>
+      <c r="F55" s="63"/>
+      <c r="G55" s="63"/>
+      <c r="H55" s="63"/>
+      <c r="I55" s="63"/>
+      <c r="J55" s="63"/>
+      <c r="K55" s="63"/>
+      <c r="L55" s="63"/>
       <c r="M55" s="32"/>
     </row>
     <row r="56" spans="1:13" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="99"/>
-      <c r="B56" s="66"/>
-      <c r="J56" s="66"/>
-      <c r="K56" s="66"/>
-      <c r="L56" s="66"/>
+      <c r="A56" s="96"/>
+      <c r="B56" s="63"/>
+      <c r="J56" s="63"/>
+      <c r="K56" s="63"/>
+      <c r="L56" s="63"/>
       <c r="M56" s="32"/>
     </row>
     <row r="57" spans="1:13" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="108"/>
-      <c r="C57" s="108"/>
-      <c r="D57" s="108"/>
-      <c r="E57" s="108"/>
-      <c r="F57" s="108"/>
-      <c r="G57" s="108"/>
-      <c r="H57" s="108"/>
-      <c r="I57" s="108"/>
-      <c r="J57" s="108"/>
+      <c r="B57" s="115"/>
+      <c r="C57" s="115"/>
+      <c r="D57" s="115"/>
+      <c r="E57" s="115"/>
+      <c r="F57" s="115"/>
+      <c r="G57" s="115"/>
+      <c r="H57" s="115"/>
+      <c r="I57" s="115"/>
+      <c r="J57" s="115"/>
       <c r="K57" s="29"/>
-      <c r="L57" s="66"/>
+      <c r="L57" s="63"/>
       <c r="M57" s="32"/>
     </row>
     <row r="58" spans="1:13" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="100" t="s">
+      <c r="A58" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="B58" s="66"/>
-      <c r="C58" s="66"/>
-      <c r="D58" s="66"/>
-      <c r="E58" s="66"/>
-      <c r="F58" s="66"/>
-      <c r="G58" s="66"/>
-      <c r="H58" s="66"/>
-      <c r="I58" s="66"/>
-      <c r="J58" s="66"/>
-      <c r="K58" s="66"/>
-      <c r="L58" s="66"/>
+      <c r="B58" s="63"/>
+      <c r="C58" s="63"/>
+      <c r="D58" s="63"/>
+      <c r="E58" s="63"/>
+      <c r="F58" s="63"/>
+      <c r="G58" s="63"/>
+      <c r="H58" s="63"/>
+      <c r="I58" s="63"/>
+      <c r="J58" s="63"/>
+      <c r="K58" s="63"/>
+      <c r="L58" s="63"/>
       <c r="M58" s="32"/>
     </row>
     <row r="59" spans="1:13" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="100" t="s">
-        <v>72</v>
-      </c>
-      <c r="B59" s="66"/>
-      <c r="C59" s="66"/>
-      <c r="D59" s="66"/>
-      <c r="E59" s="101" t="s">
+      <c r="A59" s="97" t="s">
+        <v>67</v>
+      </c>
+      <c r="B59" s="63"/>
+      <c r="C59" s="63"/>
+      <c r="D59" s="63"/>
+      <c r="E59" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="F59" s="66"/>
-      <c r="G59" s="66"/>
-      <c r="H59" s="66"/>
-      <c r="I59" s="66"/>
-      <c r="J59" s="66"/>
-      <c r="K59" s="66"/>
-      <c r="L59" s="66"/>
+      <c r="F59" s="63"/>
+      <c r="G59" s="63"/>
+      <c r="H59" s="63"/>
+      <c r="I59" s="63"/>
+      <c r="J59" s="63"/>
+      <c r="K59" s="63"/>
+      <c r="L59" s="63"/>
       <c r="M59" s="32"/>
     </row>
     <row r="60" spans="1:13" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="61" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="107" t="s">
-        <v>73</v>
-      </c>
-      <c r="B61" s="107"/>
-      <c r="C61" s="107"/>
-      <c r="D61" s="107"/>
-      <c r="E61" s="107"/>
-      <c r="F61" s="107"/>
-      <c r="G61" s="107"/>
-      <c r="H61" s="107"/>
-      <c r="I61" s="107"/>
-      <c r="J61" s="107"/>
-      <c r="K61" s="107"/>
-      <c r="L61" s="107"/>
+      <c r="A61" s="114" t="s">
+        <v>68</v>
+      </c>
+      <c r="B61" s="114"/>
+      <c r="C61" s="114"/>
+      <c r="D61" s="114"/>
+      <c r="E61" s="114"/>
+      <c r="F61" s="114"/>
+      <c r="G61" s="114"/>
+      <c r="H61" s="114"/>
+      <c r="I61" s="114"/>
+      <c r="J61" s="114"/>
+      <c r="K61" s="114"/>
+      <c r="L61" s="114"/>
     </row>
     <row r="62" spans="1:13" ht="15.9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="63" spans="1:13" ht="15.9" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3329,7 +3122,7 @@
     <protectedRange sqref="C13 C16" name="Rango3_3_1_1_1_1_1_1_1_1"/>
     <protectedRange sqref="C57" name="Rango3_3_1_1_1_1_1_2_1"/>
   </protectedRanges>
-  <mergeCells count="49">
+  <mergeCells count="50">
     <mergeCell ref="J41:L41"/>
     <mergeCell ref="B48:D48"/>
     <mergeCell ref="C31:G31"/>
@@ -3349,7 +3142,6 @@
     <mergeCell ref="B30:G30"/>
     <mergeCell ref="H25:J25"/>
     <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H27:I27"/>
     <mergeCell ref="A15:L15"/>
     <mergeCell ref="J30:K30"/>
     <mergeCell ref="A25:D25"/>
@@ -3358,6 +3150,8 @@
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="E27:F27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="E28:F28"/>
     <mergeCell ref="A7:L7"/>
     <mergeCell ref="A8:L8"/>
     <mergeCell ref="A14:L14"/>
@@ -3430,10 +3224,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="145" t="s">
+      <c r="A2" s="155" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="145"/>
+      <c r="B2" s="155"/>
       <c r="C2" s="5" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
fix: ajustar footer revisado/aprobado para mostrar fecha en humedad
</commit_message>
<xml_diff>
--- a/app/templates/Template_Humedad.xlsx
+++ b/app/templates/Template_Humedad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\crmnew\api-geofal-crm\app\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26ACD2A0-3DEE-4F31-BBF6-A5144280BE4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485D29F4-CB6A-4C94-A931-4F97A50C29C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="723" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -238,9 +238,6 @@
     <t>Fuente: Elaboración propia en base a la Norma ASTM D2216-19.</t>
   </si>
   <si>
-    <t>Versión: 04 (01-12-2022)</t>
-  </si>
-  <si>
     <t>WEB: www.geofal.com.pe   E-MAIL: laboratorio@geofal.com.pe                                                                                                                                                                         Av. Marañon 763, Los Olivos-Lima / Teléfono  01 754-3070</t>
   </si>
   <si>
@@ -278,6 +275,9 @@
   </si>
   <si>
     <t xml:space="preserve">Descripción material excluido: </t>
+  </si>
+  <si>
+    <t>Versión: 05 (16-02-2026)</t>
   </si>
 </sst>
 </file>
@@ -1415,15 +1415,8 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>Revisado: angel</a:t>
+            <a:t>Revisado: </a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="es-PE" sz="1000" b="0">
-            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -1439,7 +1432,7 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>Fecha: 04/11/26</a:t>
+            <a:t>Fecha: </a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1511,15 +1504,8 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>Aprobado: JAZMIN</a:t>
+            <a:t>Aprobado: </a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="es-PE" sz="1000" b="0">
-            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -1535,7 +1521,7 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>Fecha: 02/02/26</a:t>
+            <a:t>Fecha: </a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2036,8 +2022,8 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:W63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="Q49" sqref="Q49"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A45" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.33203125" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2188,18 +2174,18 @@
       <c r="A10" s="27"/>
       <c r="B10" s="27"/>
       <c r="D10" s="110" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="110" t="s">
         <v>69</v>
-      </c>
-      <c r="E10" s="110" t="s">
-        <v>70</v>
       </c>
       <c r="F10" s="111"/>
       <c r="G10" s="112" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H10" s="113"/>
       <c r="I10" s="110" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J10" s="27"/>
       <c r="K10" s="27"/>
@@ -2375,7 +2361,7 @@
     </row>
     <row r="22" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B22" s="40"/>
       <c r="C22" s="40"/>
@@ -2427,12 +2413,12 @@
       <c r="C25" s="148"/>
       <c r="D25" s="148"/>
       <c r="E25" s="149" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F25" s="149"/>
       <c r="G25" s="104"/>
       <c r="H25" s="140" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I25" s="141"/>
       <c r="J25" s="142"/>
@@ -2447,12 +2433,12 @@
       <c r="C26" s="148"/>
       <c r="D26" s="148"/>
       <c r="E26" s="149" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F26" s="149"/>
       <c r="G26" s="104"/>
       <c r="H26" s="143" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I26" s="143"/>
       <c r="J26" s="105"/>
@@ -2467,7 +2453,7 @@
       <c r="C27" s="148"/>
       <c r="D27" s="148"/>
       <c r="E27" s="149" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F27" s="149"/>
       <c r="G27" s="104"/>
@@ -2480,7 +2466,7 @@
     </row>
     <row r="28" spans="1:19" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="148" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B28" s="148"/>
       <c r="C28" s="148"/>
@@ -2586,7 +2572,7 @@
       <c r="F33" s="152"/>
       <c r="G33" s="153"/>
       <c r="H33" s="58" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I33" s="100"/>
       <c r="J33" s="59"/>
@@ -2608,7 +2594,7 @@
       <c r="F34" s="152"/>
       <c r="G34" s="153"/>
       <c r="H34" s="58" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I34" s="100"/>
       <c r="J34" s="59"/>
@@ -2632,7 +2618,7 @@
       <c r="F35" s="152"/>
       <c r="G35" s="153"/>
       <c r="H35" s="58" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I35" s="100"/>
       <c r="J35" s="59"/>
@@ -2656,7 +2642,7 @@
       <c r="F36" s="152"/>
       <c r="G36" s="153"/>
       <c r="H36" s="58" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I36" s="100"/>
       <c r="J36" s="59"/>
@@ -2680,7 +2666,7 @@
       <c r="F37" s="152"/>
       <c r="G37" s="153"/>
       <c r="H37" s="58" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I37" s="100"/>
       <c r="J37" s="59"/>
@@ -2704,7 +2690,7 @@
       <c r="F38" s="152"/>
       <c r="G38" s="153"/>
       <c r="H38" s="58" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I38" s="100"/>
       <c r="J38" s="59"/>
@@ -3081,7 +3067,7 @@
     </row>
     <row r="59" spans="1:13" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="97" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="B59" s="63"/>
       <c r="C59" s="63"/>
@@ -3101,7 +3087,7 @@
     <row r="60" spans="1:13" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="61" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="114" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B61" s="114"/>
       <c r="C61" s="114"/>

</xml_diff>

<commit_message>
fix(humedad): exportar excel sin dropdowns y actualizar template
</commit_message>
<xml_diff>
--- a/app/templates/Template_Humedad.xlsx
+++ b/app/templates/Template_Humedad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\crmnew\api-geofal-crm\app\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485D29F4-CB6A-4C94-A931-4F97A50C29C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A034F559-0BB7-4406-90F7-ABFE78422585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="723" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -211,9 +211,6 @@
     <t>Masa del recipiente y muestra seca al horno constante</t>
   </si>
   <si>
-    <t>Masa del agua (5-3)</t>
-  </si>
-  <si>
     <t>Masa de muestra seca al horno (5-6)</t>
   </si>
   <si>
@@ -278,6 +275,9 @@
   </si>
   <si>
     <t>Versión: 05 (16-02-2026)</t>
+  </si>
+  <si>
+    <t>Masa del agua (3-5)</t>
   </si>
 </sst>
 </file>
@@ -685,7 +685,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="156">
+  <cellXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1003,12 +1003,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
@@ -1050,6 +1044,104 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="16" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1057,10 +1149,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -1101,105 +1189,14 @@
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2022,8 +2019,8 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:W63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A45" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A23" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37:G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.33203125" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2125,36 +2122,36 @@
       <c r="L6" s="26"/>
     </row>
     <row r="7" spans="1:13" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="130" t="s">
+      <c r="A7" s="131" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="130"/>
-      <c r="C7" s="130"/>
-      <c r="D7" s="130"/>
-      <c r="E7" s="130"/>
-      <c r="F7" s="130"/>
-      <c r="G7" s="130"/>
-      <c r="H7" s="130"/>
-      <c r="I7" s="130"/>
-      <c r="J7" s="130"/>
-      <c r="K7" s="130"/>
-      <c r="L7" s="130"/>
+      <c r="B7" s="131"/>
+      <c r="C7" s="131"/>
+      <c r="D7" s="131"/>
+      <c r="E7" s="131"/>
+      <c r="F7" s="131"/>
+      <c r="G7" s="131"/>
+      <c r="H7" s="131"/>
+      <c r="I7" s="131"/>
+      <c r="J7" s="131"/>
+      <c r="K7" s="131"/>
+      <c r="L7" s="131"/>
     </row>
     <row r="8" spans="1:13" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="131" t="s">
+      <c r="A8" s="132" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="131"/>
-      <c r="C8" s="131"/>
-      <c r="D8" s="131"/>
-      <c r="E8" s="131"/>
-      <c r="F8" s="131"/>
-      <c r="G8" s="131"/>
-      <c r="H8" s="131"/>
-      <c r="I8" s="131"/>
-      <c r="J8" s="131"/>
-      <c r="K8" s="131"/>
-      <c r="L8" s="131"/>
+      <c r="B8" s="132"/>
+      <c r="C8" s="132"/>
+      <c r="D8" s="132"/>
+      <c r="E8" s="132"/>
+      <c r="F8" s="132"/>
+      <c r="G8" s="132"/>
+      <c r="H8" s="132"/>
+      <c r="I8" s="132"/>
+      <c r="J8" s="132"/>
+      <c r="K8" s="132"/>
+      <c r="L8" s="132"/>
     </row>
     <row r="9" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27"/>
@@ -2173,19 +2170,19 @@
     <row r="10" spans="1:13" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="27"/>
       <c r="B10" s="27"/>
-      <c r="D10" s="110" t="s">
+      <c r="D10" s="108" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="108" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="110" t="s">
+      <c r="F10" s="109"/>
+      <c r="G10" s="110" t="s">
         <v>69</v>
       </c>
-      <c r="F10" s="111"/>
-      <c r="G10" s="112" t="s">
+      <c r="H10" s="111"/>
+      <c r="I10" s="108" t="s">
         <v>70</v>
-      </c>
-      <c r="H10" s="113"/>
-      <c r="I10" s="110" t="s">
-        <v>71</v>
       </c>
       <c r="J10" s="27"/>
       <c r="K10" s="27"/>
@@ -2195,12 +2192,12 @@
       <c r="A11" s="27"/>
       <c r="B11" s="27"/>
       <c r="C11" s="27"/>
-      <c r="D11" s="110"/>
-      <c r="E11" s="110"/>
-      <c r="F11" s="111"/>
-      <c r="G11" s="112"/>
-      <c r="H11" s="113"/>
-      <c r="I11" s="110"/>
+      <c r="D11" s="108"/>
+      <c r="E11" s="108"/>
+      <c r="F11" s="109"/>
+      <c r="G11" s="110"/>
+      <c r="H11" s="111"/>
+      <c r="I11" s="108"/>
       <c r="J11" s="27"/>
       <c r="K11" s="27"/>
       <c r="L11" s="27"/>
@@ -2231,37 +2228,37 @@
       <c r="M13" s="32"/>
     </row>
     <row r="14" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="132" t="s">
+      <c r="A14" s="133" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="133"/>
-      <c r="C14" s="133"/>
-      <c r="D14" s="133"/>
-      <c r="E14" s="133"/>
-      <c r="F14" s="133"/>
-      <c r="G14" s="133"/>
-      <c r="H14" s="133"/>
-      <c r="I14" s="133"/>
-      <c r="J14" s="133"/>
-      <c r="K14" s="133"/>
-      <c r="L14" s="134"/>
+      <c r="B14" s="134"/>
+      <c r="C14" s="134"/>
+      <c r="D14" s="134"/>
+      <c r="E14" s="134"/>
+      <c r="F14" s="134"/>
+      <c r="G14" s="134"/>
+      <c r="H14" s="134"/>
+      <c r="I14" s="134"/>
+      <c r="J14" s="134"/>
+      <c r="K14" s="134"/>
+      <c r="L14" s="135"/>
       <c r="M14" s="32"/>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="144" t="s">
+      <c r="A15" s="125" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="145"/>
-      <c r="C15" s="145"/>
-      <c r="D15" s="145"/>
-      <c r="E15" s="145"/>
-      <c r="F15" s="145"/>
-      <c r="G15" s="145"/>
-      <c r="H15" s="145"/>
-      <c r="I15" s="145"/>
-      <c r="J15" s="145"/>
-      <c r="K15" s="145"/>
-      <c r="L15" s="146"/>
+      <c r="B15" s="126"/>
+      <c r="C15" s="126"/>
+      <c r="D15" s="126"/>
+      <c r="E15" s="126"/>
+      <c r="F15" s="126"/>
+      <c r="G15" s="126"/>
+      <c r="H15" s="126"/>
+      <c r="I15" s="126"/>
+      <c r="J15" s="126"/>
+      <c r="K15" s="126"/>
+      <c r="L15" s="127"/>
       <c r="M15" s="32"/>
     </row>
     <row r="16" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2280,17 +2277,17 @@
       <c r="M16" s="32"/>
     </row>
     <row r="17" spans="1:19" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="135" t="s">
+      <c r="A17" s="136" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="136"/>
-      <c r="C17" s="136"/>
-      <c r="D17" s="136"/>
-      <c r="E17" s="136"/>
-      <c r="F17" s="136"/>
-      <c r="G17" s="136"/>
-      <c r="H17" s="136"/>
-      <c r="I17" s="136"/>
+      <c r="B17" s="137"/>
+      <c r="C17" s="137"/>
+      <c r="D17" s="137"/>
+      <c r="E17" s="137"/>
+      <c r="F17" s="137"/>
+      <c r="G17" s="137"/>
+      <c r="H17" s="137"/>
+      <c r="I17" s="137"/>
       <c r="J17" s="37"/>
       <c r="K17" s="37"/>
       <c r="L17" s="38"/>
@@ -2361,7 +2358,7 @@
     </row>
     <row r="22" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="41" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B22" s="40"/>
       <c r="C22" s="40"/>
@@ -2390,93 +2387,93 @@
       <c r="L23" s="38"/>
     </row>
     <row r="24" spans="1:19" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="137" t="s">
+      <c r="A24" s="138" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="138"/>
-      <c r="C24" s="138"/>
-      <c r="D24" s="138"/>
-      <c r="E24" s="102"/>
-      <c r="F24" s="102"/>
-      <c r="G24" s="102"/>
-      <c r="H24" s="102"/>
-      <c r="I24" s="102"/>
-      <c r="J24" s="103"/>
+      <c r="B24" s="139"/>
+      <c r="C24" s="139"/>
+      <c r="D24" s="139"/>
+      <c r="E24" s="100"/>
+      <c r="F24" s="100"/>
+      <c r="G24" s="100"/>
+      <c r="H24" s="100"/>
+      <c r="I24" s="100"/>
+      <c r="J24" s="101"/>
       <c r="K24" s="37"/>
       <c r="L24" s="38"/>
     </row>
     <row r="25" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="148" t="s">
+      <c r="A25" s="129" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="148"/>
-      <c r="C25" s="148"/>
-      <c r="D25" s="148"/>
-      <c r="E25" s="149" t="s">
-        <v>72</v>
-      </c>
-      <c r="F25" s="149"/>
-      <c r="G25" s="104"/>
-      <c r="H25" s="140" t="s">
-        <v>76</v>
-      </c>
-      <c r="I25" s="141"/>
-      <c r="J25" s="142"/>
+      <c r="B25" s="129"/>
+      <c r="C25" s="129"/>
+      <c r="D25" s="129"/>
+      <c r="E25" s="130" t="s">
+        <v>71</v>
+      </c>
+      <c r="F25" s="130"/>
+      <c r="G25" s="102"/>
+      <c r="H25" s="121" t="s">
+        <v>75</v>
+      </c>
+      <c r="I25" s="122"/>
+      <c r="J25" s="123"/>
       <c r="K25" s="45"/>
       <c r="L25" s="38"/>
     </row>
     <row r="26" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="148" t="s">
+      <c r="A26" s="129" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="148"/>
-      <c r="C26" s="148"/>
-      <c r="D26" s="148"/>
-      <c r="E26" s="149" t="s">
-        <v>73</v>
-      </c>
-      <c r="F26" s="149"/>
-      <c r="G26" s="104"/>
-      <c r="H26" s="143" t="s">
-        <v>77</v>
-      </c>
-      <c r="I26" s="143"/>
-      <c r="J26" s="105"/>
+      <c r="B26" s="129"/>
+      <c r="C26" s="129"/>
+      <c r="D26" s="129"/>
+      <c r="E26" s="130" t="s">
+        <v>72</v>
+      </c>
+      <c r="F26" s="130"/>
+      <c r="G26" s="102"/>
+      <c r="H26" s="124" t="s">
+        <v>76</v>
+      </c>
+      <c r="I26" s="124"/>
+      <c r="J26" s="103"/>
       <c r="K26" s="46"/>
       <c r="L26" s="38"/>
     </row>
     <row r="27" spans="1:19" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="148" t="s">
-        <v>62</v>
-      </c>
-      <c r="B27" s="148"/>
-      <c r="C27" s="148"/>
-      <c r="D27" s="148"/>
-      <c r="E27" s="149" t="s">
-        <v>74</v>
-      </c>
-      <c r="F27" s="149"/>
-      <c r="G27" s="104"/>
-      <c r="H27" s="106"/>
-      <c r="I27" s="107"/>
-      <c r="J27" s="108"/>
-      <c r="K27" s="108"/>
+      <c r="A27" s="129" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="129"/>
+      <c r="C27" s="129"/>
+      <c r="D27" s="129"/>
+      <c r="E27" s="130" t="s">
+        <v>73</v>
+      </c>
+      <c r="F27" s="130"/>
+      <c r="G27" s="102"/>
+      <c r="H27" s="104"/>
+      <c r="I27" s="105"/>
+      <c r="J27" s="106"/>
+      <c r="K27" s="106"/>
       <c r="L27" s="38"/>
       <c r="M27" s="32"/>
     </row>
     <row r="28" spans="1:19" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="148" t="s">
-        <v>78</v>
-      </c>
-      <c r="B28" s="148"/>
-      <c r="C28" s="148"/>
-      <c r="D28" s="148"/>
-      <c r="E28" s="149"/>
-      <c r="F28" s="149"/>
-      <c r="G28" s="109"/>
-      <c r="H28" s="109"/>
-      <c r="I28" s="109"/>
-      <c r="J28" s="109"/>
+      <c r="A28" s="129" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" s="129"/>
+      <c r="C28" s="129"/>
+      <c r="D28" s="129"/>
+      <c r="E28" s="130"/>
+      <c r="F28" s="130"/>
+      <c r="G28" s="107"/>
+      <c r="H28" s="107"/>
+      <c r="I28" s="107"/>
+      <c r="J28" s="107"/>
       <c r="L28" s="47"/>
       <c r="M28" s="32"/>
     </row>
@@ -2497,22 +2494,22 @@
     </row>
     <row r="30" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="53"/>
-      <c r="B30" s="139" t="s">
+      <c r="B30" s="120" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="139"/>
-      <c r="D30" s="139"/>
-      <c r="E30" s="139"/>
-      <c r="F30" s="139"/>
-      <c r="G30" s="139"/>
+      <c r="C30" s="120"/>
+      <c r="D30" s="120"/>
+      <c r="E30" s="120"/>
+      <c r="F30" s="120"/>
+      <c r="G30" s="120"/>
       <c r="H30" s="54" t="s">
         <v>40</v>
       </c>
       <c r="I30" s="54" t="s">
-        <v>61</v>
-      </c>
-      <c r="J30" s="147"/>
-      <c r="K30" s="147"/>
+        <v>60</v>
+      </c>
+      <c r="J30" s="128"/>
+      <c r="K30" s="128"/>
       <c r="L30" s="55"/>
       <c r="M30" s="32"/>
     </row>
@@ -2521,17 +2518,17 @@
       <c r="B31" s="57">
         <v>1</v>
       </c>
-      <c r="C31" s="151" t="s">
+      <c r="C31" s="115" t="s">
         <v>17</v>
       </c>
-      <c r="D31" s="152"/>
-      <c r="E31" s="152"/>
-      <c r="F31" s="152"/>
-      <c r="G31" s="153"/>
+      <c r="D31" s="116"/>
+      <c r="E31" s="116"/>
+      <c r="F31" s="116"/>
+      <c r="G31" s="117"/>
       <c r="H31" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="I31" s="101"/>
+      <c r="I31" s="154"/>
       <c r="J31" s="59"/>
       <c r="K31" s="59"/>
       <c r="L31" s="60"/>
@@ -2542,17 +2539,17 @@
       <c r="B32" s="61">
         <v>2</v>
       </c>
-      <c r="C32" s="151" t="s">
+      <c r="C32" s="115" t="s">
         <v>36</v>
       </c>
-      <c r="D32" s="152"/>
-      <c r="E32" s="152"/>
-      <c r="F32" s="152"/>
-      <c r="G32" s="153"/>
+      <c r="D32" s="116"/>
+      <c r="E32" s="116"/>
+      <c r="F32" s="116"/>
+      <c r="G32" s="117"/>
       <c r="H32" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="I32" s="100"/>
+      <c r="I32" s="154"/>
       <c r="J32" s="59"/>
       <c r="K32" s="59"/>
       <c r="L32" s="60"/>
@@ -2564,17 +2561,17 @@
       <c r="B33" s="61">
         <v>3</v>
       </c>
-      <c r="C33" s="151" t="s">
+      <c r="C33" s="115" t="s">
         <v>37</v>
       </c>
-      <c r="D33" s="152"/>
-      <c r="E33" s="152"/>
-      <c r="F33" s="152"/>
-      <c r="G33" s="153"/>
+      <c r="D33" s="116"/>
+      <c r="E33" s="116"/>
+      <c r="F33" s="116"/>
+      <c r="G33" s="117"/>
       <c r="H33" s="58" t="s">
-        <v>75</v>
-      </c>
-      <c r="I33" s="100"/>
+        <v>74</v>
+      </c>
+      <c r="I33" s="154"/>
       <c r="J33" s="59"/>
       <c r="K33" s="59"/>
       <c r="L33" s="64"/>
@@ -2586,17 +2583,17 @@
       <c r="B34" s="57">
         <v>4</v>
       </c>
-      <c r="C34" s="151" t="s">
+      <c r="C34" s="115" t="s">
         <v>56</v>
       </c>
-      <c r="D34" s="152"/>
-      <c r="E34" s="152"/>
-      <c r="F34" s="152"/>
-      <c r="G34" s="153"/>
+      <c r="D34" s="116"/>
+      <c r="E34" s="116"/>
+      <c r="F34" s="116"/>
+      <c r="G34" s="117"/>
       <c r="H34" s="58" t="s">
-        <v>75</v>
-      </c>
-      <c r="I34" s="100"/>
+        <v>74</v>
+      </c>
+      <c r="I34" s="154"/>
       <c r="J34" s="59"/>
       <c r="K34" s="59"/>
       <c r="L34" s="64"/>
@@ -2610,17 +2607,17 @@
       <c r="B35" s="61">
         <v>5</v>
       </c>
-      <c r="C35" s="151" t="s">
+      <c r="C35" s="115" t="s">
         <v>57</v>
       </c>
-      <c r="D35" s="152"/>
-      <c r="E35" s="152"/>
-      <c r="F35" s="152"/>
-      <c r="G35" s="153"/>
+      <c r="D35" s="116"/>
+      <c r="E35" s="116"/>
+      <c r="F35" s="116"/>
+      <c r="G35" s="117"/>
       <c r="H35" s="58" t="s">
-        <v>75</v>
-      </c>
-      <c r="I35" s="100"/>
+        <v>74</v>
+      </c>
+      <c r="I35" s="154"/>
       <c r="J35" s="59"/>
       <c r="K35" s="59"/>
       <c r="L35" s="66"/>
@@ -2634,17 +2631,17 @@
       <c r="B36" s="57">
         <v>6</v>
       </c>
-      <c r="C36" s="151" t="s">
+      <c r="C36" s="115" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="152"/>
-      <c r="E36" s="152"/>
-      <c r="F36" s="152"/>
-      <c r="G36" s="153"/>
+      <c r="D36" s="116"/>
+      <c r="E36" s="116"/>
+      <c r="F36" s="116"/>
+      <c r="G36" s="117"/>
       <c r="H36" s="58" t="s">
-        <v>75</v>
-      </c>
-      <c r="I36" s="100"/>
+        <v>74</v>
+      </c>
+      <c r="I36" s="154"/>
       <c r="J36" s="59"/>
       <c r="K36" s="59"/>
       <c r="L36" s="66"/>
@@ -2658,17 +2655,17 @@
       <c r="B37" s="61">
         <v>7</v>
       </c>
-      <c r="C37" s="151" t="s">
-        <v>58</v>
-      </c>
-      <c r="D37" s="152"/>
-      <c r="E37" s="152"/>
-      <c r="F37" s="152"/>
-      <c r="G37" s="153"/>
+      <c r="C37" s="115" t="s">
+        <v>80</v>
+      </c>
+      <c r="D37" s="116"/>
+      <c r="E37" s="116"/>
+      <c r="F37" s="116"/>
+      <c r="G37" s="117"/>
       <c r="H37" s="58" t="s">
-        <v>75</v>
-      </c>
-      <c r="I37" s="100"/>
+        <v>74</v>
+      </c>
+      <c r="I37" s="154"/>
       <c r="J37" s="59"/>
       <c r="K37" s="59"/>
       <c r="L37" s="66"/>
@@ -2682,17 +2679,17 @@
       <c r="B38" s="61">
         <v>8</v>
       </c>
-      <c r="C38" s="151" t="s">
-        <v>59</v>
-      </c>
-      <c r="D38" s="152"/>
-      <c r="E38" s="152"/>
-      <c r="F38" s="152"/>
-      <c r="G38" s="153"/>
+      <c r="C38" s="115" t="s">
+        <v>58</v>
+      </c>
+      <c r="D38" s="116"/>
+      <c r="E38" s="116"/>
+      <c r="F38" s="116"/>
+      <c r="G38" s="117"/>
       <c r="H38" s="58" t="s">
-        <v>75</v>
-      </c>
-      <c r="I38" s="100"/>
+        <v>74</v>
+      </c>
+      <c r="I38" s="154"/>
       <c r="J38" s="59"/>
       <c r="K38" s="59"/>
       <c r="L38" s="66"/>
@@ -2706,17 +2703,17 @@
       <c r="B39" s="57">
         <v>9</v>
       </c>
-      <c r="C39" s="151" t="s">
-        <v>60</v>
-      </c>
-      <c r="D39" s="152"/>
-      <c r="E39" s="152"/>
-      <c r="F39" s="152"/>
-      <c r="G39" s="153"/>
+      <c r="C39" s="115" t="s">
+        <v>59</v>
+      </c>
+      <c r="D39" s="116"/>
+      <c r="E39" s="116"/>
+      <c r="F39" s="116"/>
+      <c r="G39" s="117"/>
       <c r="H39" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="I39" s="100"/>
+      <c r="I39" s="154"/>
       <c r="J39" s="59"/>
       <c r="K39" s="59"/>
       <c r="L39" s="66"/>
@@ -2742,187 +2739,187 @@
     </row>
     <row r="41" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="56"/>
-      <c r="B41" s="127" t="s">
+      <c r="B41" s="118" t="s">
         <v>43</v>
       </c>
-      <c r="C41" s="127"/>
-      <c r="D41" s="127"/>
-      <c r="E41" s="127"/>
-      <c r="F41" s="127"/>
+      <c r="C41" s="118"/>
+      <c r="D41" s="118"/>
+      <c r="E41" s="118"/>
+      <c r="F41" s="118"/>
       <c r="G41" s="74"/>
-      <c r="H41" s="116" t="s">
+      <c r="H41" s="142" t="s">
         <v>26</v>
       </c>
-      <c r="I41" s="117"/>
-      <c r="J41" s="150"/>
-      <c r="K41" s="150"/>
-      <c r="L41" s="117"/>
+      <c r="I41" s="113"/>
+      <c r="J41" s="112"/>
+      <c r="K41" s="112"/>
+      <c r="L41" s="113"/>
       <c r="M41" s="32"/>
       <c r="W41" s="63"/>
     </row>
     <row r="42" spans="1:23" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="56"/>
-      <c r="B42" s="128" t="s">
+      <c r="B42" s="152" t="s">
         <v>49</v>
       </c>
-      <c r="C42" s="128"/>
-      <c r="D42" s="128"/>
+      <c r="C42" s="152"/>
+      <c r="D42" s="152"/>
       <c r="E42" s="75" t="s">
         <v>48</v>
       </c>
       <c r="F42" s="75" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G42" s="74"/>
-      <c r="H42" s="126" t="s">
+      <c r="H42" s="151" t="s">
         <v>27</v>
       </c>
-      <c r="I42" s="126"/>
-      <c r="J42" s="125"/>
-      <c r="K42" s="125"/>
-      <c r="L42" s="125"/>
+      <c r="I42" s="151"/>
+      <c r="J42" s="150"/>
+      <c r="K42" s="150"/>
+      <c r="L42" s="150"/>
       <c r="M42" s="32"/>
       <c r="W42" s="63"/>
     </row>
     <row r="43" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="56"/>
-      <c r="B43" s="129" t="s">
+      <c r="B43" s="114" t="s">
         <v>52</v>
       </c>
-      <c r="C43" s="129"/>
-      <c r="D43" s="129"/>
+      <c r="C43" s="114"/>
+      <c r="D43" s="114"/>
       <c r="E43" s="76" t="s">
         <v>23</v>
       </c>
       <c r="F43" s="76" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G43" s="74"/>
-      <c r="H43" s="126" t="s">
+      <c r="H43" s="151" t="s">
         <v>28</v>
       </c>
-      <c r="I43" s="126"/>
-      <c r="J43" s="118"/>
-      <c r="K43" s="118"/>
-      <c r="L43" s="119"/>
+      <c r="I43" s="151"/>
+      <c r="J43" s="143"/>
+      <c r="K43" s="143"/>
+      <c r="L43" s="144"/>
       <c r="M43" s="32"/>
       <c r="W43" s="63"/>
     </row>
     <row r="44" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="56"/>
-      <c r="B44" s="129" t="s">
+      <c r="B44" s="114" t="s">
         <v>53</v>
       </c>
-      <c r="C44" s="129"/>
-      <c r="D44" s="129"/>
+      <c r="C44" s="114"/>
+      <c r="D44" s="114"/>
       <c r="E44" s="76" t="s">
         <v>22</v>
       </c>
       <c r="F44" s="76" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G44" s="74"/>
-      <c r="H44" s="126"/>
-      <c r="I44" s="126"/>
-      <c r="J44" s="120"/>
-      <c r="K44" s="120"/>
-      <c r="L44" s="121"/>
+      <c r="H44" s="151"/>
+      <c r="I44" s="151"/>
+      <c r="J44" s="145"/>
+      <c r="K44" s="145"/>
+      <c r="L44" s="146"/>
       <c r="M44" s="32"/>
     </row>
     <row r="45" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="56"/>
-      <c r="B45" s="154" t="s">
+      <c r="B45" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="C45" s="154"/>
-      <c r="D45" s="154"/>
+      <c r="C45" s="119"/>
+      <c r="D45" s="119"/>
       <c r="E45" s="76" t="s">
         <v>21</v>
       </c>
       <c r="F45" s="76" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G45" s="74"/>
-      <c r="H45" s="126" t="s">
+      <c r="H45" s="151" t="s">
         <v>29</v>
       </c>
-      <c r="I45" s="126"/>
-      <c r="J45" s="118"/>
-      <c r="K45" s="118"/>
-      <c r="L45" s="119"/>
+      <c r="I45" s="151"/>
+      <c r="J45" s="143"/>
+      <c r="K45" s="143"/>
+      <c r="L45" s="144"/>
       <c r="M45" s="32"/>
     </row>
     <row r="46" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="56"/>
-      <c r="B46" s="127" t="s">
+      <c r="B46" s="118" t="s">
         <v>44</v>
       </c>
-      <c r="C46" s="127"/>
-      <c r="D46" s="127"/>
-      <c r="E46" s="127"/>
-      <c r="F46" s="127"/>
+      <c r="C46" s="118"/>
+      <c r="D46" s="118"/>
+      <c r="E46" s="118"/>
+      <c r="F46" s="118"/>
       <c r="G46" s="74"/>
-      <c r="H46" s="126"/>
-      <c r="I46" s="126"/>
-      <c r="J46" s="120"/>
-      <c r="K46" s="120"/>
-      <c r="L46" s="121"/>
+      <c r="H46" s="151"/>
+      <c r="I46" s="151"/>
+      <c r="J46" s="145"/>
+      <c r="K46" s="145"/>
+      <c r="L46" s="146"/>
       <c r="M46" s="32"/>
     </row>
     <row r="47" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="56"/>
-      <c r="B47" s="154" t="s">
+      <c r="B47" s="119" t="s">
         <v>55</v>
       </c>
-      <c r="C47" s="154"/>
-      <c r="D47" s="154"/>
+      <c r="C47" s="119"/>
+      <c r="D47" s="119"/>
       <c r="E47" s="76" t="s">
         <v>20</v>
       </c>
       <c r="F47" s="76" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G47" s="74"/>
-      <c r="H47" s="122"/>
-      <c r="I47" s="122"/>
-      <c r="J47" s="123"/>
-      <c r="K47" s="123"/>
-      <c r="L47" s="124"/>
+      <c r="H47" s="147"/>
+      <c r="I47" s="147"/>
+      <c r="J47" s="148"/>
+      <c r="K47" s="148"/>
+      <c r="L47" s="149"/>
       <c r="M47" s="32"/>
     </row>
     <row r="48" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="56"/>
-      <c r="B48" s="129" t="s">
+      <c r="B48" s="114" t="s">
         <v>50</v>
       </c>
-      <c r="C48" s="129"/>
-      <c r="D48" s="129"/>
+      <c r="C48" s="114"/>
+      <c r="D48" s="114"/>
       <c r="E48" s="76" t="s">
         <v>21</v>
       </c>
       <c r="F48" s="76" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G48" s="74"/>
-      <c r="H48" s="122"/>
-      <c r="I48" s="122"/>
-      <c r="J48" s="123"/>
-      <c r="K48" s="123"/>
-      <c r="L48" s="124"/>
+      <c r="H48" s="147"/>
+      <c r="I48" s="147"/>
+      <c r="J48" s="148"/>
+      <c r="K48" s="148"/>
+      <c r="L48" s="149"/>
       <c r="M48" s="32"/>
     </row>
     <row r="49" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="56"/>
-      <c r="B49" s="129" t="s">
+      <c r="B49" s="114" t="s">
         <v>51</v>
       </c>
-      <c r="C49" s="129"/>
-      <c r="D49" s="129"/>
+      <c r="C49" s="114"/>
+      <c r="D49" s="114"/>
       <c r="E49" s="76" t="s">
         <v>21</v>
       </c>
       <c r="F49" s="76" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G49" s="74"/>
       <c r="H49" s="77"/>
@@ -2935,7 +2932,7 @@
     <row r="50" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="80"/>
       <c r="B50" s="81" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C50" s="82"/>
       <c r="D50" s="82"/>
@@ -3035,15 +3032,15 @@
       <c r="M56" s="32"/>
     </row>
     <row r="57" spans="1:13" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="115"/>
-      <c r="C57" s="115"/>
-      <c r="D57" s="115"/>
-      <c r="E57" s="115"/>
-      <c r="F57" s="115"/>
-      <c r="G57" s="115"/>
-      <c r="H57" s="115"/>
-      <c r="I57" s="115"/>
-      <c r="J57" s="115"/>
+      <c r="B57" s="141"/>
+      <c r="C57" s="141"/>
+      <c r="D57" s="141"/>
+      <c r="E57" s="141"/>
+      <c r="F57" s="141"/>
+      <c r="G57" s="141"/>
+      <c r="H57" s="141"/>
+      <c r="I57" s="141"/>
+      <c r="J57" s="141"/>
       <c r="K57" s="29"/>
       <c r="L57" s="63"/>
       <c r="M57" s="32"/>
@@ -3067,7 +3064,7 @@
     </row>
     <row r="59" spans="1:13" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="97" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B59" s="63"/>
       <c r="C59" s="63"/>
@@ -3086,20 +3083,20 @@
     </row>
     <row r="60" spans="1:13" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="61" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="114" t="s">
-        <v>67</v>
-      </c>
-      <c r="B61" s="114"/>
-      <c r="C61" s="114"/>
-      <c r="D61" s="114"/>
-      <c r="E61" s="114"/>
-      <c r="F61" s="114"/>
-      <c r="G61" s="114"/>
-      <c r="H61" s="114"/>
-      <c r="I61" s="114"/>
-      <c r="J61" s="114"/>
-      <c r="K61" s="114"/>
-      <c r="L61" s="114"/>
+      <c r="A61" s="140" t="s">
+        <v>66</v>
+      </c>
+      <c r="B61" s="140"/>
+      <c r="C61" s="140"/>
+      <c r="D61" s="140"/>
+      <c r="E61" s="140"/>
+      <c r="F61" s="140"/>
+      <c r="G61" s="140"/>
+      <c r="H61" s="140"/>
+      <c r="I61" s="140"/>
+      <c r="J61" s="140"/>
+      <c r="K61" s="140"/>
+      <c r="L61" s="140"/>
     </row>
     <row r="62" spans="1:13" ht="15.9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="63" spans="1:13" ht="15.9" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3109,6 +3106,40 @@
     <protectedRange sqref="C57" name="Rango3_3_1_1_1_1_1_2_1"/>
   </protectedRanges>
   <mergeCells count="50">
+    <mergeCell ref="A61:L61"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="E57:H57"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="J43:L44"/>
+    <mergeCell ref="J45:L46"/>
+    <mergeCell ref="H47:I48"/>
+    <mergeCell ref="J47:L48"/>
+    <mergeCell ref="J42:L42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="H45:I46"/>
+    <mergeCell ref="H43:I44"/>
+    <mergeCell ref="A7:L7"/>
+    <mergeCell ref="A8:L8"/>
+    <mergeCell ref="A14:L14"/>
+    <mergeCell ref="A17:I17"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="H25:J25"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="A15:L15"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="E28:F28"/>
     <mergeCell ref="J41:L41"/>
     <mergeCell ref="B48:D48"/>
     <mergeCell ref="C31:G31"/>
@@ -3125,40 +3156,6 @@
     <mergeCell ref="C36:G36"/>
     <mergeCell ref="C37:G37"/>
     <mergeCell ref="C38:G38"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="H25:J25"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="A15:L15"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="A7:L7"/>
-    <mergeCell ref="A8:L8"/>
-    <mergeCell ref="A14:L14"/>
-    <mergeCell ref="A17:I17"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A61:L61"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="E57:H57"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="J43:L44"/>
-    <mergeCell ref="J45:L46"/>
-    <mergeCell ref="H47:I48"/>
-    <mergeCell ref="J47:L48"/>
-    <mergeCell ref="J42:L42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="H45:I46"/>
-    <mergeCell ref="H43:I44"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="A18:A22">
@@ -3210,10 +3207,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="155" t="s">
+      <c r="A2" s="153" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="155"/>
+      <c r="B2" s="153"/>
       <c r="C2" s="5" t="s">
         <v>10</v>
       </c>

</xml_diff>